<commit_message>
Make fingering font larger. Fix mistake in fingering
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23117"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16380" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="MoonlightSonanta.txt" sheetId="1" r:id="rId1"/>
@@ -322,8 +322,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="39">
+  <cellStyleXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -367,7 +369,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="39">
+  <cellStyles count="41">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -387,6 +389,7 @@
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -406,6 +409,7 @@
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -738,8 +742,8 @@
   <dimension ref="A1:J1147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H18" sqref="H18"/>
+      <pane ySplit="1" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1733,10 +1737,10 @@
         <v>70</v>
       </c>
       <c r="B31" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C31" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="D31">
         <v>8</v>
@@ -1745,7 +1749,7 @@
         <v>80</v>
       </c>
       <c r="F31">
-        <v>0.33333299999999999</v>
+        <v>1.9895799999999999</v>
       </c>
       <c r="G31" t="s">
         <v>80</v>
@@ -1757,7 +1761,7 @@
         <v>71</v>
       </c>
       <c r="J31">
-        <f t="shared" si="0"/>
+        <f>FLOOR(D31/4+1,1)</f>
         <v>3</v>
       </c>
     </row>
@@ -1766,10 +1770,10 @@
         <v>70</v>
       </c>
       <c r="B32" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C32" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D32">
         <v>8</v>
@@ -1778,7 +1782,7 @@
         <v>80</v>
       </c>
       <c r="F32">
-        <v>1.9895799999999999</v>
+        <v>0.33333299999999999</v>
       </c>
       <c r="G32" t="s">
         <v>80</v>

</xml_diff>

<commit_message>
Fingering complete to measure 13
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -325,8 +325,30 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="79">
+  <cellStyleXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -410,7 +432,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="79">
+  <cellStyles count="101">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -450,6 +472,17 @@
     <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -489,6 +522,17 @@
     <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -821,8 +865,8 @@
   <dimension ref="A1:K1147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H1152" sqref="H1152"/>
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H213" sqref="H213"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5631,6 +5675,9 @@
       <c r="G134" t="s">
         <v>80</v>
       </c>
+      <c r="H134">
+        <v>-5</v>
+      </c>
       <c r="I134" t="s">
         <v>71</v>
       </c>
@@ -5664,6 +5711,9 @@
       <c r="G135" t="s">
         <v>80</v>
       </c>
+      <c r="H135">
+        <v>-1</v>
+      </c>
       <c r="I135" t="s">
         <v>71</v>
       </c>
@@ -5697,6 +5747,9 @@
       <c r="G136" t="s">
         <v>80</v>
       </c>
+      <c r="H136">
+        <v>1</v>
+      </c>
       <c r="I136" t="s">
         <v>71</v>
       </c>
@@ -5730,6 +5783,9 @@
       <c r="G137" t="s">
         <v>80</v>
       </c>
+      <c r="H137">
+        <v>2</v>
+      </c>
       <c r="I137" t="s">
         <v>71</v>
       </c>
@@ -5763,6 +5819,9 @@
       <c r="G138" t="s">
         <v>80</v>
       </c>
+      <c r="H138">
+        <v>4</v>
+      </c>
       <c r="I138" t="s">
         <v>71</v>
       </c>
@@ -5829,6 +5888,9 @@
       <c r="G140" t="s">
         <v>80</v>
       </c>
+      <c r="H140">
+        <v>1</v>
+      </c>
       <c r="I140" t="s">
         <v>71</v>
       </c>
@@ -5862,6 +5924,9 @@
       <c r="G141" t="s">
         <v>80</v>
       </c>
+      <c r="H141">
+        <v>2</v>
+      </c>
       <c r="I141" t="s">
         <v>71</v>
       </c>
@@ -5895,6 +5960,9 @@
       <c r="G142" t="s">
         <v>80</v>
       </c>
+      <c r="H142">
+        <v>4</v>
+      </c>
       <c r="I142" t="s">
         <v>71</v>
       </c>
@@ -5928,6 +5996,9 @@
       <c r="G143" t="s">
         <v>80</v>
       </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
       <c r="I143" t="s">
         <v>71</v>
       </c>
@@ -5961,6 +6032,9 @@
       <c r="G144" t="s">
         <v>80</v>
       </c>
+      <c r="H144">
+        <v>2</v>
+      </c>
       <c r="I144" t="s">
         <v>71</v>
       </c>
@@ -5994,6 +6068,9 @@
       <c r="G145" t="s">
         <v>80</v>
       </c>
+      <c r="H145">
+        <v>4</v>
+      </c>
       <c r="I145" t="s">
         <v>71</v>
       </c>
@@ -6027,6 +6104,9 @@
       <c r="G146" t="s">
         <v>80</v>
       </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
       <c r="I146" t="s">
         <v>71</v>
       </c>
@@ -6060,6 +6140,9 @@
       <c r="G147" t="s">
         <v>80</v>
       </c>
+      <c r="H147">
+        <v>2</v>
+      </c>
       <c r="I147" t="s">
         <v>71</v>
       </c>
@@ -6093,6 +6176,9 @@
       <c r="G148" t="s">
         <v>80</v>
       </c>
+      <c r="H148">
+        <v>4</v>
+      </c>
       <c r="I148" t="s">
         <v>71</v>
       </c>
@@ -6126,6 +6212,9 @@
       <c r="G149" t="s">
         <v>80</v>
       </c>
+      <c r="H149">
+        <v>-5</v>
+      </c>
       <c r="I149" t="s">
         <v>71</v>
       </c>
@@ -6159,6 +6248,9 @@
       <c r="G150" t="s">
         <v>80</v>
       </c>
+      <c r="H150">
+        <v>-1</v>
+      </c>
       <c r="I150" t="s">
         <v>71</v>
       </c>
@@ -6192,6 +6284,9 @@
       <c r="G151" t="s">
         <v>80</v>
       </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
       <c r="I151" t="s">
         <v>71</v>
       </c>
@@ -6225,6 +6320,9 @@
       <c r="G152" t="s">
         <v>80</v>
       </c>
+      <c r="H152">
+        <v>2</v>
+      </c>
       <c r="I152" t="s">
         <v>71</v>
       </c>
@@ -6258,6 +6356,9 @@
       <c r="G153" t="s">
         <v>80</v>
       </c>
+      <c r="H153">
+        <v>4</v>
+      </c>
       <c r="I153" t="s">
         <v>71</v>
       </c>
@@ -6291,6 +6392,9 @@
       <c r="G154" t="s">
         <v>80</v>
       </c>
+      <c r="H154">
+        <v>1</v>
+      </c>
       <c r="I154" t="s">
         <v>71</v>
       </c>
@@ -6324,6 +6428,9 @@
       <c r="G155" t="s">
         <v>80</v>
       </c>
+      <c r="H155">
+        <v>2</v>
+      </c>
       <c r="I155" t="s">
         <v>71</v>
       </c>
@@ -6357,6 +6464,9 @@
       <c r="G156" t="s">
         <v>80</v>
       </c>
+      <c r="H156">
+        <v>4</v>
+      </c>
       <c r="I156" t="s">
         <v>71</v>
       </c>
@@ -6390,6 +6500,9 @@
       <c r="G157" t="s">
         <v>80</v>
       </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
       <c r="I157" t="s">
         <v>71</v>
       </c>
@@ -6423,6 +6536,9 @@
       <c r="G158" t="s">
         <v>80</v>
       </c>
+      <c r="H158">
+        <v>2</v>
+      </c>
       <c r="I158" t="s">
         <v>71</v>
       </c>
@@ -6456,6 +6572,9 @@
       <c r="G159" t="s">
         <v>80</v>
       </c>
+      <c r="H159">
+        <v>4</v>
+      </c>
       <c r="I159" t="s">
         <v>71</v>
       </c>
@@ -6489,6 +6608,9 @@
       <c r="G160" t="s">
         <v>80</v>
       </c>
+      <c r="H160">
+        <v>1</v>
+      </c>
       <c r="I160" t="s">
         <v>71</v>
       </c>
@@ -6522,6 +6644,9 @@
       <c r="G161" t="s">
         <v>80</v>
       </c>
+      <c r="H161">
+        <v>5</v>
+      </c>
       <c r="I161" t="s">
         <v>71</v>
       </c>
@@ -6555,6 +6680,9 @@
       <c r="G162" t="s">
         <v>80</v>
       </c>
+      <c r="H162">
+        <v>2</v>
+      </c>
       <c r="I162" t="s">
         <v>71</v>
       </c>
@@ -6588,6 +6716,9 @@
       <c r="G163" t="s">
         <v>80</v>
       </c>
+      <c r="H163">
+        <v>4</v>
+      </c>
       <c r="I163" t="s">
         <v>71</v>
       </c>
@@ -6621,6 +6752,9 @@
       <c r="G164" t="s">
         <v>80</v>
       </c>
+      <c r="H164">
+        <v>5</v>
+      </c>
       <c r="I164" t="s">
         <v>71</v>
       </c>
@@ -6654,6 +6788,9 @@
       <c r="G165" t="s">
         <v>80</v>
       </c>
+      <c r="H165">
+        <v>-5</v>
+      </c>
       <c r="I165" t="s">
         <v>71</v>
       </c>
@@ -6687,6 +6824,9 @@
       <c r="G166" t="s">
         <v>80</v>
       </c>
+      <c r="H166">
+        <v>-1</v>
+      </c>
       <c r="I166" t="s">
         <v>71</v>
       </c>
@@ -6720,6 +6860,9 @@
       <c r="G167" t="s">
         <v>80</v>
       </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
       <c r="I167" t="s">
         <v>71</v>
       </c>
@@ -6753,6 +6896,9 @@
       <c r="G168" t="s">
         <v>80</v>
       </c>
+      <c r="H168">
+        <v>5</v>
+      </c>
       <c r="I168" t="s">
         <v>71</v>
       </c>
@@ -6786,6 +6932,9 @@
       <c r="G169" t="s">
         <v>80</v>
       </c>
+      <c r="H169">
+        <v>2</v>
+      </c>
       <c r="I169" t="s">
         <v>71</v>
       </c>
@@ -6819,6 +6968,9 @@
       <c r="G170" t="s">
         <v>80</v>
       </c>
+      <c r="H170">
+        <v>4</v>
+      </c>
       <c r="I170" t="s">
         <v>71</v>
       </c>
@@ -6852,6 +7004,9 @@
       <c r="G171" t="s">
         <v>80</v>
       </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
       <c r="I171" t="s">
         <v>71</v>
       </c>
@@ -6885,6 +7040,9 @@
       <c r="G172" t="s">
         <v>80</v>
       </c>
+      <c r="H172">
+        <v>2</v>
+      </c>
       <c r="I172" t="s">
         <v>71</v>
       </c>
@@ -6918,6 +7076,9 @@
       <c r="G173" t="s">
         <v>80</v>
       </c>
+      <c r="H173">
+        <v>4</v>
+      </c>
       <c r="I173" t="s">
         <v>71</v>
       </c>
@@ -6951,6 +7112,9 @@
       <c r="G174" t="s">
         <v>80</v>
       </c>
+      <c r="H174">
+        <v>1</v>
+      </c>
       <c r="I174" t="s">
         <v>71</v>
       </c>
@@ -6984,6 +7148,9 @@
       <c r="G175" t="s">
         <v>80</v>
       </c>
+      <c r="H175">
+        <v>2</v>
+      </c>
       <c r="I175" t="s">
         <v>71</v>
       </c>
@@ -7017,6 +7184,9 @@
       <c r="G176" t="s">
         <v>80</v>
       </c>
+      <c r="H176">
+        <v>4</v>
+      </c>
       <c r="I176" t="s">
         <v>71</v>
       </c>
@@ -7050,6 +7220,9 @@
       <c r="G177" t="s">
         <v>80</v>
       </c>
+      <c r="H177">
+        <v>1</v>
+      </c>
       <c r="I177" t="s">
         <v>71</v>
       </c>
@@ -7083,6 +7256,9 @@
       <c r="G178" t="s">
         <v>80</v>
       </c>
+      <c r="H178">
+        <v>5</v>
+      </c>
       <c r="I178" t="s">
         <v>71</v>
       </c>
@@ -7116,6 +7292,9 @@
       <c r="G179" t="s">
         <v>80</v>
       </c>
+      <c r="H179">
+        <v>2</v>
+      </c>
       <c r="I179" t="s">
         <v>71</v>
       </c>
@@ -7149,6 +7328,9 @@
       <c r="G180" t="s">
         <v>80</v>
       </c>
+      <c r="H180">
+        <v>4</v>
+      </c>
       <c r="I180" t="s">
         <v>71</v>
       </c>
@@ -7182,6 +7364,9 @@
       <c r="G181" t="s">
         <v>80</v>
       </c>
+      <c r="H181">
+        <v>5</v>
+      </c>
       <c r="I181" t="s">
         <v>71</v>
       </c>
@@ -7215,6 +7400,9 @@
       <c r="G182" t="s">
         <v>80</v>
       </c>
+      <c r="H182">
+        <v>-5</v>
+      </c>
       <c r="I182" t="s">
         <v>71</v>
       </c>
@@ -7248,6 +7436,9 @@
       <c r="G183" t="s">
         <v>80</v>
       </c>
+      <c r="H183">
+        <v>-1</v>
+      </c>
       <c r="I183" t="s">
         <v>71</v>
       </c>
@@ -7281,6 +7472,9 @@
       <c r="G184" t="s">
         <v>80</v>
       </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
       <c r="I184" t="s">
         <v>71</v>
       </c>
@@ -7314,6 +7508,9 @@
       <c r="G185" t="s">
         <v>80</v>
       </c>
+      <c r="H185">
+        <v>5</v>
+      </c>
       <c r="I185" t="s">
         <v>71</v>
       </c>
@@ -7347,6 +7544,9 @@
       <c r="G186" t="s">
         <v>80</v>
       </c>
+      <c r="H186">
+        <v>2</v>
+      </c>
       <c r="I186" t="s">
         <v>71</v>
       </c>
@@ -7380,6 +7580,9 @@
       <c r="G187" t="s">
         <v>80</v>
       </c>
+      <c r="H187">
+        <v>4</v>
+      </c>
       <c r="I187" t="s">
         <v>71</v>
       </c>
@@ -7413,6 +7616,9 @@
       <c r="G188" t="s">
         <v>80</v>
       </c>
+      <c r="H188">
+        <v>-5</v>
+      </c>
       <c r="I188" t="s">
         <v>71</v>
       </c>
@@ -7446,6 +7652,9 @@
       <c r="G189" t="s">
         <v>80</v>
       </c>
+      <c r="H189">
+        <v>-1</v>
+      </c>
       <c r="I189" t="s">
         <v>71</v>
       </c>
@@ -7479,6 +7688,9 @@
       <c r="G190" t="s">
         <v>80</v>
       </c>
+      <c r="H190">
+        <v>1</v>
+      </c>
       <c r="I190" t="s">
         <v>71</v>
       </c>
@@ -7512,6 +7724,9 @@
       <c r="G191" t="s">
         <v>80</v>
       </c>
+      <c r="H191">
+        <v>2</v>
+      </c>
       <c r="I191" t="s">
         <v>71</v>
       </c>
@@ -7545,6 +7760,9 @@
       <c r="G192" t="s">
         <v>80</v>
       </c>
+      <c r="H192">
+        <v>4</v>
+      </c>
       <c r="I192" t="s">
         <v>71</v>
       </c>
@@ -7578,6 +7796,9 @@
       <c r="G193" t="s">
         <v>80</v>
       </c>
+      <c r="H193">
+        <v>-5</v>
+      </c>
       <c r="I193" t="s">
         <v>71</v>
       </c>
@@ -7611,6 +7832,9 @@
       <c r="G194" t="s">
         <v>80</v>
       </c>
+      <c r="H194">
+        <v>-1</v>
+      </c>
       <c r="I194" t="s">
         <v>71</v>
       </c>
@@ -7644,6 +7868,9 @@
       <c r="G195" t="s">
         <v>80</v>
       </c>
+      <c r="H195">
+        <v>1</v>
+      </c>
       <c r="I195" t="s">
         <v>71</v>
       </c>
@@ -7677,6 +7904,9 @@
       <c r="G196" t="s">
         <v>80</v>
       </c>
+      <c r="H196">
+        <v>2</v>
+      </c>
       <c r="I196" t="s">
         <v>71</v>
       </c>
@@ -7710,6 +7940,9 @@
       <c r="G197" t="s">
         <v>80</v>
       </c>
+      <c r="H197">
+        <v>4</v>
+      </c>
       <c r="I197" t="s">
         <v>71</v>
       </c>
@@ -7743,6 +7976,9 @@
       <c r="G198" t="s">
         <v>80</v>
       </c>
+      <c r="H198">
+        <v>1</v>
+      </c>
       <c r="I198" t="s">
         <v>71</v>
       </c>
@@ -7776,6 +8012,9 @@
       <c r="G199" t="s">
         <v>80</v>
       </c>
+      <c r="H199">
+        <v>5</v>
+      </c>
       <c r="I199" t="s">
         <v>71</v>
       </c>
@@ -7809,6 +8048,9 @@
       <c r="G200" t="s">
         <v>80</v>
       </c>
+      <c r="H200">
+        <v>2</v>
+      </c>
       <c r="I200" t="s">
         <v>71</v>
       </c>
@@ -7842,6 +8084,9 @@
       <c r="G201" t="s">
         <v>80</v>
       </c>
+      <c r="H201">
+        <v>4</v>
+      </c>
       <c r="I201" t="s">
         <v>71</v>
       </c>
@@ -7875,6 +8120,9 @@
       <c r="G202" t="s">
         <v>80</v>
       </c>
+      <c r="H202">
+        <v>-5</v>
+      </c>
       <c r="I202" t="s">
         <v>71</v>
       </c>
@@ -7908,6 +8156,9 @@
       <c r="G203" t="s">
         <v>80</v>
       </c>
+      <c r="H203">
+        <v>-1</v>
+      </c>
       <c r="I203" t="s">
         <v>71</v>
       </c>
@@ -7941,6 +8192,9 @@
       <c r="G204" t="s">
         <v>80</v>
       </c>
+      <c r="H204">
+        <v>1</v>
+      </c>
       <c r="I204" t="s">
         <v>71</v>
       </c>
@@ -7974,6 +8228,9 @@
       <c r="G205" t="s">
         <v>80</v>
       </c>
+      <c r="H205">
+        <v>5</v>
+      </c>
       <c r="I205" t="s">
         <v>71</v>
       </c>
@@ -8007,6 +8264,9 @@
       <c r="G206" t="s">
         <v>80</v>
       </c>
+      <c r="H206">
+        <v>2</v>
+      </c>
       <c r="I206" t="s">
         <v>71</v>
       </c>
@@ -8040,6 +8300,9 @@
       <c r="G207" t="s">
         <v>80</v>
       </c>
+      <c r="H207">
+        <v>3</v>
+      </c>
       <c r="I207" t="s">
         <v>71</v>
       </c>
@@ -8073,6 +8336,9 @@
       <c r="G208" t="s">
         <v>80</v>
       </c>
+      <c r="H208">
+        <v>1</v>
+      </c>
       <c r="I208" t="s">
         <v>71</v>
       </c>
@@ -8106,6 +8372,9 @@
       <c r="G209" t="s">
         <v>80</v>
       </c>
+      <c r="H209">
+        <v>2</v>
+      </c>
       <c r="I209" t="s">
         <v>71</v>
       </c>
@@ -8139,6 +8408,9 @@
       <c r="G210" t="s">
         <v>80</v>
       </c>
+      <c r="H210">
+        <v>3</v>
+      </c>
       <c r="I210" t="s">
         <v>71</v>
       </c>
@@ -8172,6 +8444,9 @@
       <c r="G211" t="s">
         <v>80</v>
       </c>
+      <c r="H211">
+        <v>-3</v>
+      </c>
       <c r="I211" t="s">
         <v>71</v>
       </c>
@@ -8205,6 +8480,9 @@
       <c r="G212" t="s">
         <v>80</v>
       </c>
+      <c r="H212">
+        <v>1</v>
+      </c>
       <c r="I212" t="s">
         <v>71</v>
       </c>
@@ -8238,6 +8516,9 @@
       <c r="G213" t="s">
         <v>80</v>
       </c>
+      <c r="H213">
+        <v>5</v>
+      </c>
       <c r="I213" t="s">
         <v>71</v>
       </c>
@@ -8271,6 +8552,9 @@
       <c r="G214" t="s">
         <v>80</v>
       </c>
+      <c r="H214">
+        <v>2</v>
+      </c>
       <c r="I214" t="s">
         <v>71</v>
       </c>
@@ -8304,6 +8588,9 @@
       <c r="G215" t="s">
         <v>80</v>
       </c>
+      <c r="H215">
+        <v>3</v>
+      </c>
       <c r="I215" t="s">
         <v>71</v>
       </c>
@@ -8337,6 +8624,9 @@
       <c r="G216" t="s">
         <v>80</v>
       </c>
+      <c r="H216">
+        <v>-1</v>
+      </c>
       <c r="I216" t="s">
         <v>71</v>
       </c>
@@ -8370,6 +8660,9 @@
       <c r="G217" t="s">
         <v>80</v>
       </c>
+      <c r="H217">
+        <v>1</v>
+      </c>
       <c r="I217" t="s">
         <v>71</v>
       </c>
@@ -8403,6 +8696,9 @@
       <c r="G218" t="s">
         <v>80</v>
       </c>
+      <c r="H218">
+        <v>5</v>
+      </c>
       <c r="I218" t="s">
         <v>71</v>
       </c>
@@ -8436,6 +8732,9 @@
       <c r="G219" t="s">
         <v>80</v>
       </c>
+      <c r="H219">
+        <v>3</v>
+      </c>
       <c r="I219" t="s">
         <v>71</v>
       </c>
@@ -8468,6 +8767,9 @@
       </c>
       <c r="G220" t="s">
         <v>80</v>
+      </c>
+      <c r="H220">
+        <v>4</v>
       </c>
       <c r="I220" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Make green key lighter so as to see fingering better. Add measure 14 fingering
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -325,8 +325,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="101">
+  <cellStyleXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -432,7 +434,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="101">
+  <cellStyles count="103">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -483,6 +485,7 @@
     <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -533,6 +536,7 @@
     <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -865,8 +869,8 @@
   <dimension ref="A1:K1147"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H213" sqref="H213"/>
+      <pane ySplit="1" topLeftCell="A204" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H238" sqref="H238"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8804,6 +8808,9 @@
       <c r="G221" t="s">
         <v>80</v>
       </c>
+      <c r="H221">
+        <v>-1</v>
+      </c>
       <c r="I221" t="s">
         <v>71</v>
       </c>
@@ -8837,6 +8844,9 @@
       <c r="G222" t="s">
         <v>80</v>
       </c>
+      <c r="H222">
+        <v>1</v>
+      </c>
       <c r="I222" t="s">
         <v>71</v>
       </c>
@@ -8870,6 +8880,9 @@
       <c r="G223" t="s">
         <v>80</v>
       </c>
+      <c r="H223">
+        <v>5</v>
+      </c>
       <c r="I223" t="s">
         <v>71</v>
       </c>
@@ -8903,6 +8916,9 @@
       <c r="G224" t="s">
         <v>80</v>
       </c>
+      <c r="H224">
+        <v>2</v>
+      </c>
       <c r="I224" t="s">
         <v>71</v>
       </c>
@@ -8936,6 +8952,9 @@
       <c r="G225" t="s">
         <v>80</v>
       </c>
+      <c r="H225">
+        <v>3</v>
+      </c>
       <c r="I225" t="s">
         <v>71</v>
       </c>
@@ -8969,6 +8988,9 @@
       <c r="G226" t="s">
         <v>80</v>
       </c>
+      <c r="H226">
+        <v>1</v>
+      </c>
       <c r="I226" t="s">
         <v>71</v>
       </c>
@@ -9002,6 +9024,9 @@
       <c r="G227" t="s">
         <v>80</v>
       </c>
+      <c r="H227">
+        <v>2</v>
+      </c>
       <c r="I227" t="s">
         <v>71</v>
       </c>
@@ -9035,6 +9060,9 @@
       <c r="G228" t="s">
         <v>80</v>
       </c>
+      <c r="H228">
+        <v>3</v>
+      </c>
       <c r="I228" t="s">
         <v>71</v>
       </c>
@@ -9068,6 +9096,9 @@
       <c r="G229" t="s">
         <v>80</v>
       </c>
+      <c r="H229">
+        <v>-5</v>
+      </c>
       <c r="I229" t="s">
         <v>71</v>
       </c>
@@ -9101,6 +9132,9 @@
       <c r="G230" t="s">
         <v>80</v>
       </c>
+      <c r="H230">
+        <v>-1</v>
+      </c>
       <c r="I230" t="s">
         <v>71</v>
       </c>
@@ -9134,6 +9168,9 @@
       <c r="G231" t="s">
         <v>80</v>
       </c>
+      <c r="H231">
+        <v>1</v>
+      </c>
       <c r="I231" t="s">
         <v>71</v>
       </c>
@@ -9167,6 +9204,9 @@
       <c r="G232" t="s">
         <v>80</v>
       </c>
+      <c r="H232">
+        <v>5</v>
+      </c>
       <c r="I232" t="s">
         <v>71</v>
       </c>
@@ -9200,6 +9240,9 @@
       <c r="G233" t="s">
         <v>80</v>
       </c>
+      <c r="H233">
+        <v>2</v>
+      </c>
       <c r="I233" t="s">
         <v>71</v>
       </c>
@@ -9233,6 +9276,9 @@
       <c r="G234" t="s">
         <v>80</v>
       </c>
+      <c r="H234">
+        <v>3</v>
+      </c>
       <c r="I234" t="s">
         <v>71</v>
       </c>
@@ -9266,6 +9312,9 @@
       <c r="G235" t="s">
         <v>80</v>
       </c>
+      <c r="H235">
+        <v>1</v>
+      </c>
       <c r="I235" t="s">
         <v>71</v>
       </c>
@@ -9299,6 +9348,9 @@
       <c r="G236" t="s">
         <v>80</v>
       </c>
+      <c r="H236">
+        <v>2</v>
+      </c>
       <c r="I236" t="s">
         <v>71</v>
       </c>
@@ -9331,6 +9383,9 @@
       </c>
       <c r="G237" t="s">
         <v>80</v>
+      </c>
+      <c r="H237">
+        <v>3</v>
       </c>
       <c r="I237" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Correct fingering mistake in measure 7
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -328,8 +328,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="153">
+  <cellStyleXfs count="169">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -487,7 +503,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="153">
+  <cellStyles count="169">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -564,6 +580,14 @@
     <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -640,6 +664,14 @@
     <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -972,8 +1004,8 @@
   <dimension ref="A1:Q1182"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A118" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B143" sqref="B143"/>
+      <pane ySplit="1" topLeftCell="A77" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I98" sqref="I98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6119,7 +6151,7 @@
         <v>4</v>
       </c>
       <c r="J98">
-        <v>-1</v>
+        <v>-5</v>
       </c>
       <c r="K98" t="s">
         <v>71</v>
@@ -6172,7 +6204,7 @@
         <v>17</v>
       </c>
       <c r="J99">
-        <v>-5</v>
+        <v>-1</v>
       </c>
       <c r="K99" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Fingering to measure 31
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -328,8 +328,64 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="191">
+  <cellStyleXfs count="247">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -525,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="191">
+  <cellStyles count="247">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -621,6 +677,34 @@
     <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -716,6 +800,34 @@
     <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1048,8 +1160,8 @@
   <dimension ref="A1:Q1181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A355" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J379" sqref="J379"/>
+      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J529" sqref="J529"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -21087,6 +21199,9 @@
       <c r="I379" t="s">
         <v>22</v>
       </c>
+      <c r="J379">
+        <v>-5</v>
+      </c>
       <c r="K379" t="s">
         <v>71</v>
       </c>
@@ -21137,6 +21252,9 @@
       <c r="I380" t="s">
         <v>34</v>
       </c>
+      <c r="J380">
+        <v>-2</v>
+      </c>
       <c r="K380" t="s">
         <v>71</v>
       </c>
@@ -21187,6 +21305,9 @@
       <c r="I381" t="s">
         <v>29</v>
       </c>
+      <c r="J381">
+        <v>-1</v>
+      </c>
       <c r="K381" t="s">
         <v>71</v>
       </c>
@@ -21237,6 +21358,9 @@
       <c r="I382" t="s">
         <v>24</v>
       </c>
+      <c r="J382">
+        <v>1</v>
+      </c>
       <c r="K382" t="s">
         <v>71</v>
       </c>
@@ -21287,6 +21411,9 @@
       <c r="I383" t="s">
         <v>11</v>
       </c>
+      <c r="J383">
+        <v>2</v>
+      </c>
       <c r="K383" t="s">
         <v>71</v>
       </c>
@@ -21337,6 +21464,9 @@
       <c r="I384" t="s">
         <v>44</v>
       </c>
+      <c r="J384">
+        <v>3</v>
+      </c>
       <c r="K384" t="s">
         <v>71</v>
       </c>
@@ -21387,6 +21517,9 @@
       <c r="I385" t="s">
         <v>0</v>
       </c>
+      <c r="J385">
+        <v>1</v>
+      </c>
       <c r="K385" t="s">
         <v>71</v>
       </c>
@@ -21437,6 +21570,9 @@
       <c r="I386" t="s">
         <v>16</v>
       </c>
+      <c r="J386">
+        <v>2</v>
+      </c>
       <c r="K386" t="s">
         <v>71</v>
       </c>
@@ -21487,6 +21623,9 @@
       <c r="I387" t="s">
         <v>22</v>
       </c>
+      <c r="J387">
+        <v>3</v>
+      </c>
       <c r="K387" t="s">
         <v>71</v>
       </c>
@@ -21537,6 +21676,9 @@
       <c r="I388" t="s">
         <v>3</v>
       </c>
+      <c r="J388">
+        <v>1</v>
+      </c>
       <c r="K388" t="s">
         <v>71</v>
       </c>
@@ -21587,6 +21729,9 @@
       <c r="I389" t="s">
         <v>23</v>
       </c>
+      <c r="J389">
+        <v>2</v>
+      </c>
       <c r="K389" t="s">
         <v>71</v>
       </c>
@@ -21637,6 +21782,9 @@
       <c r="I390" t="s">
         <v>22</v>
       </c>
+      <c r="J390">
+        <v>3</v>
+      </c>
       <c r="K390" t="s">
         <v>71</v>
       </c>
@@ -21687,6 +21835,9 @@
       <c r="I391" t="s">
         <v>7</v>
       </c>
+      <c r="J391">
+        <v>1</v>
+      </c>
       <c r="K391" t="s">
         <v>71</v>
       </c>
@@ -21737,6 +21888,9 @@
       <c r="I392" t="s">
         <v>50</v>
       </c>
+      <c r="J392">
+        <v>5</v>
+      </c>
       <c r="K392" t="s">
         <v>71</v>
       </c>
@@ -21787,6 +21941,9 @@
       <c r="I393" t="s">
         <v>10</v>
       </c>
+      <c r="J393">
+        <v>2</v>
+      </c>
       <c r="K393" t="s">
         <v>71</v>
       </c>
@@ -21837,6 +21994,9 @@
       <c r="I394" t="s">
         <v>1</v>
       </c>
+      <c r="J394">
+        <v>3</v>
+      </c>
       <c r="K394" t="s">
         <v>71</v>
       </c>
@@ -21886,6 +22046,9 @@
       </c>
       <c r="I395" t="s">
         <v>32</v>
+      </c>
+      <c r="J395">
+        <v>5</v>
       </c>
       <c r="K395" t="s">
         <v>71</v>
@@ -21937,6 +22100,9 @@
       <c r="I396" t="s">
         <v>1</v>
       </c>
+      <c r="J396">
+        <v>-5</v>
+      </c>
       <c r="K396" t="s">
         <v>71</v>
       </c>
@@ -21987,6 +22153,9 @@
       <c r="I397" t="s">
         <v>16</v>
       </c>
+      <c r="J397">
+        <v>-2</v>
+      </c>
       <c r="K397" t="s">
         <v>71</v>
       </c>
@@ -22037,6 +22206,9 @@
       <c r="I398" t="s">
         <v>17</v>
       </c>
+      <c r="J398">
+        <v>-1</v>
+      </c>
       <c r="K398" t="s">
         <v>71</v>
       </c>
@@ -22087,6 +22259,9 @@
       <c r="I399" t="s">
         <v>17</v>
       </c>
+      <c r="J399">
+        <v>1</v>
+      </c>
       <c r="K399" t="s">
         <v>71</v>
       </c>
@@ -22137,6 +22312,9 @@
       <c r="I400" t="s">
         <v>5</v>
       </c>
+      <c r="J400">
+        <v>5</v>
+      </c>
       <c r="K400" t="s">
         <v>71</v>
       </c>
@@ -22187,6 +22365,9 @@
       <c r="I401" t="s">
         <v>14</v>
       </c>
+      <c r="J401">
+        <v>3</v>
+      </c>
       <c r="K401" t="s">
         <v>71</v>
       </c>
@@ -22237,6 +22418,9 @@
       <c r="I402" t="s">
         <v>4</v>
       </c>
+      <c r="J402">
+        <v>4</v>
+      </c>
       <c r="K402" t="s">
         <v>71</v>
       </c>
@@ -22287,6 +22471,9 @@
       <c r="I403" t="s">
         <v>14</v>
       </c>
+      <c r="J403">
+        <v>1</v>
+      </c>
       <c r="K403" t="s">
         <v>71</v>
       </c>
@@ -22337,6 +22524,9 @@
       <c r="I404" t="s">
         <v>29</v>
       </c>
+      <c r="J404">
+        <v>3</v>
+      </c>
       <c r="K404" t="s">
         <v>71</v>
       </c>
@@ -22387,6 +22577,9 @@
       <c r="I405" t="s">
         <v>18</v>
       </c>
+      <c r="J405">
+        <v>4</v>
+      </c>
       <c r="K405" t="s">
         <v>71</v>
       </c>
@@ -22437,6 +22630,9 @@
       <c r="I406" t="s">
         <v>17</v>
       </c>
+      <c r="J406">
+        <v>1</v>
+      </c>
       <c r="K406" t="s">
         <v>71</v>
       </c>
@@ -22487,6 +22683,9 @@
       <c r="I407" t="s">
         <v>10</v>
       </c>
+      <c r="J407">
+        <v>3</v>
+      </c>
       <c r="K407" t="s">
         <v>71</v>
       </c>
@@ -22537,6 +22736,9 @@
       <c r="I408" t="s">
         <v>45</v>
       </c>
+      <c r="J408">
+        <v>4</v>
+      </c>
       <c r="K408" t="s">
         <v>71</v>
       </c>
@@ -22587,6 +22789,9 @@
       <c r="I409" t="s">
         <v>10</v>
       </c>
+      <c r="J409">
+        <v>1</v>
+      </c>
       <c r="K409" t="s">
         <v>71</v>
       </c>
@@ -22637,6 +22842,9 @@
       <c r="I410" t="s">
         <v>19</v>
       </c>
+      <c r="J410">
+        <v>5</v>
+      </c>
       <c r="K410" t="s">
         <v>71</v>
       </c>
@@ -22687,6 +22895,9 @@
       <c r="I411" t="s">
         <v>18</v>
       </c>
+      <c r="J411">
+        <v>3</v>
+      </c>
       <c r="K411" t="s">
         <v>71</v>
       </c>
@@ -22737,6 +22948,9 @@
       <c r="I412" t="s">
         <v>17</v>
       </c>
+      <c r="J412">
+        <v>4</v>
+      </c>
       <c r="K412" t="s">
         <v>71</v>
       </c>
@@ -22786,6 +23000,9 @@
       </c>
       <c r="I413" t="s">
         <v>3</v>
+      </c>
+      <c r="J413">
+        <v>5</v>
       </c>
       <c r="K413" t="s">
         <v>71</v>
@@ -22837,6 +23054,9 @@
       <c r="I414" t="s">
         <v>18</v>
       </c>
+      <c r="J414">
+        <v>-5</v>
+      </c>
       <c r="K414" t="s">
         <v>71</v>
       </c>
@@ -22887,6 +23107,9 @@
       <c r="I415" t="s">
         <v>36</v>
       </c>
+      <c r="J415">
+        <v>-1</v>
+      </c>
       <c r="K415" t="s">
         <v>71</v>
       </c>
@@ -22937,6 +23160,9 @@
       <c r="I416" t="s">
         <v>18</v>
       </c>
+      <c r="J416">
+        <v>1</v>
+      </c>
       <c r="K416" t="s">
         <v>71</v>
       </c>
@@ -22987,6 +23213,9 @@
       <c r="I417" t="s">
         <v>5</v>
       </c>
+      <c r="J417">
+        <v>5</v>
+      </c>
       <c r="K417" t="s">
         <v>71</v>
       </c>
@@ -23037,6 +23266,9 @@
       <c r="I418" t="s">
         <v>17</v>
       </c>
+      <c r="J418">
+        <v>2</v>
+      </c>
       <c r="K418" t="s">
         <v>71</v>
       </c>
@@ -23087,6 +23319,9 @@
       <c r="I419" t="s">
         <v>44</v>
       </c>
+      <c r="J419">
+        <v>3</v>
+      </c>
       <c r="K419" t="s">
         <v>71</v>
       </c>
@@ -23137,6 +23372,9 @@
       <c r="I420" t="s">
         <v>3</v>
       </c>
+      <c r="J420">
+        <v>1</v>
+      </c>
       <c r="K420" t="s">
         <v>71</v>
       </c>
@@ -23187,6 +23425,9 @@
       <c r="I421" t="s">
         <v>10</v>
       </c>
+      <c r="J421">
+        <v>2</v>
+      </c>
       <c r="K421" t="s">
         <v>71</v>
       </c>
@@ -23237,6 +23478,9 @@
       <c r="I422" t="s">
         <v>17</v>
       </c>
+      <c r="J422">
+        <v>3</v>
+      </c>
       <c r="K422" t="s">
         <v>71</v>
       </c>
@@ -23287,6 +23531,9 @@
       <c r="I423" t="s">
         <v>2</v>
       </c>
+      <c r="J423">
+        <v>-5</v>
+      </c>
       <c r="K423" t="s">
         <v>71</v>
       </c>
@@ -23337,6 +23584,9 @@
       <c r="I424" t="s">
         <v>47</v>
       </c>
+      <c r="J424">
+        <v>-1</v>
+      </c>
       <c r="K424" t="s">
         <v>71</v>
       </c>
@@ -23387,6 +23637,9 @@
       <c r="I425" t="s">
         <v>31</v>
       </c>
+      <c r="J425">
+        <v>1</v>
+      </c>
       <c r="K425" t="s">
         <v>71</v>
       </c>
@@ -23437,6 +23690,9 @@
       <c r="I426" t="s">
         <v>40</v>
       </c>
+      <c r="J426">
+        <v>5</v>
+      </c>
       <c r="K426" t="s">
         <v>71</v>
       </c>
@@ -23487,6 +23743,9 @@
       <c r="I427" t="s">
         <v>12</v>
       </c>
+      <c r="J427">
+        <v>2</v>
+      </c>
       <c r="K427" t="s">
         <v>71</v>
       </c>
@@ -23537,6 +23796,9 @@
       <c r="I428" t="s">
         <v>44</v>
       </c>
+      <c r="J428">
+        <v>3</v>
+      </c>
       <c r="K428" t="s">
         <v>71</v>
       </c>
@@ -23587,6 +23849,9 @@
       <c r="I429" t="s">
         <v>53</v>
       </c>
+      <c r="J429">
+        <v>-5</v>
+      </c>
       <c r="K429" t="s">
         <v>71</v>
       </c>
@@ -23637,6 +23902,9 @@
       <c r="I430" t="s">
         <v>25</v>
       </c>
+      <c r="J430">
+        <v>-1</v>
+      </c>
       <c r="K430" t="s">
         <v>71</v>
       </c>
@@ -23687,6 +23955,9 @@
       <c r="I431" t="s">
         <v>46</v>
       </c>
+      <c r="J431">
+        <v>1</v>
+      </c>
       <c r="K431" t="s">
         <v>71</v>
       </c>
@@ -23737,6 +24008,9 @@
       <c r="I432" t="s">
         <v>58</v>
       </c>
+      <c r="J432">
+        <v>5</v>
+      </c>
       <c r="K432" t="s">
         <v>71</v>
       </c>
@@ -23787,6 +24061,9 @@
       <c r="I433" t="s">
         <v>4</v>
       </c>
+      <c r="J433">
+        <v>2</v>
+      </c>
       <c r="K433" t="s">
         <v>71</v>
       </c>
@@ -23836,6 +24113,9 @@
       </c>
       <c r="I434" t="s">
         <v>4</v>
+      </c>
+      <c r="J434">
+        <v>3</v>
       </c>
       <c r="K434" t="s">
         <v>71</v>
@@ -23887,6 +24167,9 @@
       <c r="I435" t="s">
         <v>47</v>
       </c>
+      <c r="J435">
+        <v>-5</v>
+      </c>
       <c r="K435" t="s">
         <v>71</v>
       </c>
@@ -23937,6 +24220,9 @@
       <c r="I436" t="s">
         <v>21</v>
       </c>
+      <c r="J436">
+        <v>-2</v>
+      </c>
       <c r="K436" t="s">
         <v>71</v>
       </c>
@@ -23987,6 +24273,9 @@
       <c r="I437" t="s">
         <v>47</v>
       </c>
+      <c r="J437">
+        <v>-1</v>
+      </c>
       <c r="K437" t="s">
         <v>71</v>
       </c>
@@ -24037,6 +24326,9 @@
       <c r="I438" t="s">
         <v>7</v>
       </c>
+      <c r="J438">
+        <v>1</v>
+      </c>
       <c r="K438" t="s">
         <v>71</v>
       </c>
@@ -24087,6 +24379,9 @@
       <c r="I439" t="s">
         <v>64</v>
       </c>
+      <c r="J439">
+        <v>5</v>
+      </c>
       <c r="K439" t="s">
         <v>71</v>
       </c>
@@ -24137,6 +24432,9 @@
       <c r="I440" t="s">
         <v>14</v>
       </c>
+      <c r="J440">
+        <v>2</v>
+      </c>
       <c r="K440" t="s">
         <v>71</v>
       </c>
@@ -24187,6 +24485,9 @@
       <c r="I441" t="s">
         <v>24</v>
       </c>
+      <c r="J441">
+        <v>3</v>
+      </c>
       <c r="K441" t="s">
         <v>71</v>
       </c>
@@ -24237,6 +24538,9 @@
       <c r="I442" t="s">
         <v>33</v>
       </c>
+      <c r="J442">
+        <v>1</v>
+      </c>
       <c r="K442" t="s">
         <v>71</v>
       </c>
@@ -24287,6 +24591,9 @@
       <c r="I443" t="s">
         <v>11</v>
       </c>
+      <c r="J443">
+        <v>2</v>
+      </c>
       <c r="K443" t="s">
         <v>71</v>
       </c>
@@ -24337,6 +24644,9 @@
       <c r="I444" t="s">
         <v>3</v>
       </c>
+      <c r="J444">
+        <v>3</v>
+      </c>
       <c r="K444" t="s">
         <v>71</v>
       </c>
@@ -24387,6 +24697,9 @@
       <c r="I445" t="s">
         <v>8</v>
       </c>
+      <c r="J445">
+        <v>1</v>
+      </c>
       <c r="K445" t="s">
         <v>71</v>
       </c>
@@ -24437,6 +24750,9 @@
       <c r="I446" t="s">
         <v>12</v>
       </c>
+      <c r="J446">
+        <v>2</v>
+      </c>
       <c r="K446" t="s">
         <v>71</v>
       </c>
@@ -24487,6 +24803,9 @@
       <c r="I447" t="s">
         <v>17</v>
       </c>
+      <c r="J447">
+        <v>3</v>
+      </c>
       <c r="K447" t="s">
         <v>71</v>
       </c>
@@ -24537,6 +24856,9 @@
       <c r="I448" t="s">
         <v>19</v>
       </c>
+      <c r="J448">
+        <v>-5</v>
+      </c>
       <c r="K448" t="s">
         <v>71</v>
       </c>
@@ -24587,6 +24909,9 @@
       <c r="I449" t="s">
         <v>4</v>
       </c>
+      <c r="J449">
+        <v>-2</v>
+      </c>
       <c r="K449" t="s">
         <v>71</v>
       </c>
@@ -24637,6 +24962,9 @@
       <c r="I450" t="s">
         <v>2</v>
       </c>
+      <c r="J450">
+        <v>-1</v>
+      </c>
       <c r="K450" t="s">
         <v>71</v>
       </c>
@@ -24687,6 +25015,9 @@
       <c r="I451" t="s">
         <v>46</v>
       </c>
+      <c r="J451">
+        <v>1</v>
+      </c>
       <c r="K451" t="s">
         <v>71</v>
       </c>
@@ -24737,6 +25068,9 @@
       <c r="I452" t="s">
         <v>50</v>
       </c>
+      <c r="J452">
+        <v>5</v>
+      </c>
       <c r="K452" t="s">
         <v>71</v>
       </c>
@@ -24787,6 +25121,9 @@
       <c r="I453" t="s">
         <v>17</v>
       </c>
+      <c r="J453">
+        <v>2</v>
+      </c>
       <c r="K453" t="s">
         <v>71</v>
       </c>
@@ -24836,6 +25173,9 @@
       </c>
       <c r="I454" t="s">
         <v>24</v>
+      </c>
+      <c r="J454">
+        <v>3</v>
       </c>
       <c r="K454" t="s">
         <v>71</v>
@@ -24887,6 +25227,9 @@
       <c r="I455" t="s">
         <v>23</v>
       </c>
+      <c r="J455">
+        <v>-5</v>
+      </c>
       <c r="K455" t="s">
         <v>71</v>
       </c>
@@ -24937,6 +25280,9 @@
       <c r="I456" t="s">
         <v>3</v>
       </c>
+      <c r="J456">
+        <v>-2</v>
+      </c>
       <c r="K456" t="s">
         <v>71</v>
       </c>
@@ -24987,6 +25333,9 @@
       <c r="I457" t="s">
         <v>8</v>
       </c>
+      <c r="J457">
+        <v>-1</v>
+      </c>
       <c r="K457" t="s">
         <v>71</v>
       </c>
@@ -25037,6 +25386,9 @@
       <c r="I458" t="s">
         <v>2</v>
       </c>
+      <c r="J458">
+        <v>1</v>
+      </c>
       <c r="K458" t="s">
         <v>71</v>
       </c>
@@ -25076,7 +25428,7 @@
         <v>77</v>
       </c>
       <c r="F459">
-        <v>2.9895800000000001</v>
+        <v>1.9895799999999999</v>
       </c>
       <c r="G459" t="s">
         <v>77</v>
@@ -25086,6 +25438,9 @@
       </c>
       <c r="I459" t="s">
         <v>50</v>
+      </c>
+      <c r="J459">
+        <v>5</v>
       </c>
       <c r="K459" t="s">
         <v>71</v>
@@ -25137,6 +25492,9 @@
       <c r="I460" t="s">
         <v>24</v>
       </c>
+      <c r="J460">
+        <v>2</v>
+      </c>
       <c r="K460" t="s">
         <v>71</v>
       </c>
@@ -25187,6 +25545,9 @@
       <c r="I461" t="s">
         <v>4</v>
       </c>
+      <c r="J461">
+        <v>4</v>
+      </c>
       <c r="K461" t="s">
         <v>71</v>
       </c>
@@ -25237,6 +25598,9 @@
       <c r="I462" t="s">
         <v>6</v>
       </c>
+      <c r="J462">
+        <v>1</v>
+      </c>
       <c r="K462" t="s">
         <v>71</v>
       </c>
@@ -25287,6 +25651,9 @@
       <c r="I463" t="s">
         <v>11</v>
       </c>
+      <c r="J463">
+        <v>2</v>
+      </c>
       <c r="K463" t="s">
         <v>71</v>
       </c>
@@ -25337,6 +25704,9 @@
       <c r="I464" t="s">
         <v>10</v>
       </c>
+      <c r="J464">
+        <v>4</v>
+      </c>
       <c r="K464" t="s">
         <v>71</v>
       </c>
@@ -25387,6 +25757,9 @@
       <c r="I465" t="s">
         <v>12</v>
       </c>
+      <c r="J465">
+        <v>-5</v>
+      </c>
       <c r="K465" t="s">
         <v>71</v>
       </c>
@@ -25437,6 +25810,9 @@
       <c r="I466" t="s">
         <v>16</v>
       </c>
+      <c r="J466">
+        <v>-1</v>
+      </c>
       <c r="K466" t="s">
         <v>71</v>
       </c>
@@ -25487,6 +25863,9 @@
       <c r="I467" t="s">
         <v>21</v>
       </c>
+      <c r="J467">
+        <v>1</v>
+      </c>
       <c r="K467" t="s">
         <v>71</v>
       </c>
@@ -25537,6 +25916,9 @@
       <c r="I468" t="s">
         <v>2</v>
       </c>
+      <c r="J468">
+        <v>5</v>
+      </c>
       <c r="K468" t="s">
         <v>71</v>
       </c>
@@ -25587,6 +25969,9 @@
       <c r="I469" t="s">
         <v>27</v>
       </c>
+      <c r="J469">
+        <v>2</v>
+      </c>
       <c r="K469" t="s">
         <v>71</v>
       </c>
@@ -25637,6 +26022,9 @@
       <c r="I470" t="s">
         <v>3</v>
       </c>
+      <c r="J470">
+        <v>3</v>
+      </c>
       <c r="K470" t="s">
         <v>71</v>
       </c>
@@ -25687,6 +26075,9 @@
       <c r="I471" t="s">
         <v>17</v>
       </c>
+      <c r="J471">
+        <v>-5</v>
+      </c>
       <c r="K471" t="s">
         <v>71</v>
       </c>
@@ -25737,6 +26128,9 @@
       <c r="I472" t="s">
         <v>3</v>
       </c>
+      <c r="J472">
+        <v>-1</v>
+      </c>
       <c r="K472" t="s">
         <v>71</v>
       </c>
@@ -25787,6 +26181,9 @@
       <c r="I473" t="s">
         <v>9</v>
       </c>
+      <c r="J473">
+        <v>1</v>
+      </c>
       <c r="K473" t="s">
         <v>71</v>
       </c>
@@ -25837,6 +26234,9 @@
       <c r="I474" t="s">
         <v>50</v>
       </c>
+      <c r="J474">
+        <v>5</v>
+      </c>
       <c r="K474" t="s">
         <v>71</v>
       </c>
@@ -25887,6 +26287,9 @@
       <c r="I475" t="s">
         <v>2</v>
       </c>
+      <c r="J475">
+        <v>2</v>
+      </c>
       <c r="K475" t="s">
         <v>71</v>
       </c>
@@ -25936,6 +26339,9 @@
       </c>
       <c r="I476" t="s">
         <v>47</v>
+      </c>
+      <c r="J476">
+        <v>4</v>
       </c>
       <c r="K476" t="s">
         <v>71</v>
@@ -25987,6 +26393,9 @@
       <c r="I477" t="s">
         <v>9</v>
       </c>
+      <c r="J477">
+        <v>-5</v>
+      </c>
       <c r="K477" t="s">
         <v>71</v>
       </c>
@@ -26037,6 +26446,9 @@
       <c r="I478" t="s">
         <v>16</v>
       </c>
+      <c r="J478">
+        <v>-1</v>
+      </c>
       <c r="K478" t="s">
         <v>71</v>
       </c>
@@ -26087,6 +26499,9 @@
       <c r="I479" t="s">
         <v>20</v>
       </c>
+      <c r="J479">
+        <v>5</v>
+      </c>
       <c r="K479" t="s">
         <v>71</v>
       </c>
@@ -26137,6 +26552,9 @@
       <c r="I480" t="s">
         <v>45</v>
       </c>
+      <c r="J480">
+        <v>1</v>
+      </c>
       <c r="K480" t="s">
         <v>71</v>
       </c>
@@ -26187,6 +26605,9 @@
       <c r="I481" t="s">
         <v>12</v>
       </c>
+      <c r="J481">
+        <v>2</v>
+      </c>
       <c r="K481" t="s">
         <v>71</v>
       </c>
@@ -26237,6 +26658,9 @@
       <c r="I482" t="s">
         <v>52</v>
       </c>
+      <c r="J482">
+        <v>4</v>
+      </c>
       <c r="K482" t="s">
         <v>71</v>
       </c>
@@ -26287,6 +26711,9 @@
       <c r="I483" t="s">
         <v>12</v>
       </c>
+      <c r="J483">
+        <v>1</v>
+      </c>
       <c r="K483" t="s">
         <v>71</v>
       </c>
@@ -26337,6 +26764,9 @@
       <c r="I484" t="s">
         <v>13</v>
       </c>
+      <c r="J484">
+        <v>2</v>
+      </c>
       <c r="K484" t="s">
         <v>71</v>
       </c>
@@ -26387,6 +26817,9 @@
       <c r="I485" t="s">
         <v>26</v>
       </c>
+      <c r="J485">
+        <v>4</v>
+      </c>
       <c r="K485" t="s">
         <v>71</v>
       </c>
@@ -26437,6 +26870,9 @@
       <c r="I486" t="s">
         <v>1</v>
       </c>
+      <c r="J486">
+        <v>1</v>
+      </c>
       <c r="K486" t="s">
         <v>71</v>
       </c>
@@ -26487,6 +26923,9 @@
       <c r="I487" t="s">
         <v>18</v>
       </c>
+      <c r="J487">
+        <v>2</v>
+      </c>
       <c r="K487" t="s">
         <v>71</v>
       </c>
@@ -26537,6 +26976,9 @@
       <c r="I488" t="s">
         <v>8</v>
       </c>
+      <c r="J488">
+        <v>3</v>
+      </c>
       <c r="K488" t="s">
         <v>71</v>
       </c>
@@ -26587,6 +27029,9 @@
       <c r="I489" t="s">
         <v>1</v>
       </c>
+      <c r="J489">
+        <v>1</v>
+      </c>
       <c r="K489" t="s">
         <v>71</v>
       </c>
@@ -26636,6 +27081,9 @@
       </c>
       <c r="I490" t="s">
         <v>4</v>
+      </c>
+      <c r="J490">
+        <v>2</v>
       </c>
       <c r="K490" t="s">
         <v>71</v>
@@ -26687,6 +27135,9 @@
       <c r="I491" t="s">
         <v>22</v>
       </c>
+      <c r="J491">
+        <v>-5</v>
+      </c>
       <c r="K491" t="s">
         <v>71</v>
       </c>
@@ -26737,6 +27188,9 @@
       <c r="I492" t="s">
         <v>10</v>
       </c>
+      <c r="J492">
+        <v>-1</v>
+      </c>
       <c r="K492" t="s">
         <v>71</v>
       </c>
@@ -26787,6 +27241,9 @@
       <c r="I493" t="s">
         <v>15</v>
       </c>
+      <c r="J493">
+        <v>1</v>
+      </c>
       <c r="K493" t="s">
         <v>71</v>
       </c>
@@ -26837,6 +27294,9 @@
       <c r="I494" t="s">
         <v>9</v>
       </c>
+      <c r="J494">
+        <v>2</v>
+      </c>
       <c r="K494" t="s">
         <v>71</v>
       </c>
@@ -26887,6 +27347,9 @@
       <c r="I495" t="s">
         <v>54</v>
       </c>
+      <c r="J495">
+        <v>4</v>
+      </c>
       <c r="K495" t="s">
         <v>71</v>
       </c>
@@ -26937,6 +27400,9 @@
       <c r="I496" t="s">
         <v>3</v>
       </c>
+      <c r="J496">
+        <v>1</v>
+      </c>
       <c r="K496" t="s">
         <v>71</v>
       </c>
@@ -26987,6 +27453,9 @@
       <c r="I497" t="s">
         <v>2</v>
       </c>
+      <c r="J497">
+        <v>2</v>
+      </c>
       <c r="K497" t="s">
         <v>71</v>
       </c>
@@ -27037,6 +27506,9 @@
       <c r="I498" t="s">
         <v>61</v>
       </c>
+      <c r="J498">
+        <v>4</v>
+      </c>
       <c r="K498" t="s">
         <v>71</v>
       </c>
@@ -27087,6 +27559,9 @@
       <c r="I499" t="s">
         <v>52</v>
       </c>
+      <c r="J499">
+        <v>1</v>
+      </c>
       <c r="K499" t="s">
         <v>71</v>
       </c>
@@ -27137,6 +27612,9 @@
       <c r="I500" t="s">
         <v>8</v>
       </c>
+      <c r="J500">
+        <v>2</v>
+      </c>
       <c r="K500" t="s">
         <v>71</v>
       </c>
@@ -27187,6 +27665,9 @@
       <c r="I501" t="s">
         <v>53</v>
       </c>
+      <c r="J501">
+        <v>3</v>
+      </c>
       <c r="K501" t="s">
         <v>71</v>
       </c>
@@ -27237,6 +27718,9 @@
       <c r="I502" t="s">
         <v>42</v>
       </c>
+      <c r="J502">
+        <v>1</v>
+      </c>
       <c r="K502" t="s">
         <v>71</v>
       </c>
@@ -27286,6 +27770,9 @@
       </c>
       <c r="I503" t="s">
         <v>14</v>
+      </c>
+      <c r="J503">
+        <v>2</v>
       </c>
       <c r="K503" t="s">
         <v>71</v>
@@ -27337,6 +27824,9 @@
       <c r="I504" t="s">
         <v>22</v>
       </c>
+      <c r="J504">
+        <v>-5</v>
+      </c>
       <c r="K504" t="s">
         <v>71</v>
       </c>
@@ -27387,6 +27877,9 @@
       <c r="I505" t="s">
         <v>4</v>
       </c>
+      <c r="J505">
+        <v>-1</v>
+      </c>
       <c r="K505" t="s">
         <v>71</v>
       </c>
@@ -27437,6 +27930,9 @@
       <c r="I506" t="s">
         <v>32</v>
       </c>
+      <c r="J506">
+        <v>1</v>
+      </c>
       <c r="K506" t="s">
         <v>71</v>
       </c>
@@ -27487,6 +27983,9 @@
       <c r="I507" t="s">
         <v>44</v>
       </c>
+      <c r="J507">
+        <v>5</v>
+      </c>
       <c r="K507" t="s">
         <v>71</v>
       </c>
@@ -27537,6 +28036,9 @@
       <c r="I508" t="s">
         <v>16</v>
       </c>
+      <c r="J508">
+        <v>2</v>
+      </c>
       <c r="K508" t="s">
         <v>71</v>
       </c>
@@ -27587,6 +28089,9 @@
       <c r="I509" t="s">
         <v>7</v>
       </c>
+      <c r="J509">
+        <v>4</v>
+      </c>
       <c r="K509" t="s">
         <v>71</v>
       </c>
@@ -27637,6 +28142,9 @@
       <c r="I510" t="s">
         <v>18</v>
       </c>
+      <c r="J510">
+        <v>1</v>
+      </c>
       <c r="K510" t="s">
         <v>71</v>
       </c>
@@ -27687,6 +28195,9 @@
       <c r="I511" t="s">
         <v>16</v>
       </c>
+      <c r="J511">
+        <v>2</v>
+      </c>
       <c r="K511" t="s">
         <v>71</v>
       </c>
@@ -27737,6 +28248,9 @@
       <c r="I512" t="s">
         <v>59</v>
       </c>
+      <c r="J512">
+        <v>5</v>
+      </c>
       <c r="K512" t="s">
         <v>71</v>
       </c>
@@ -27787,6 +28301,9 @@
       <c r="I513" t="s">
         <v>11</v>
       </c>
+      <c r="J513">
+        <v>1</v>
+      </c>
       <c r="K513" t="s">
         <v>71</v>
       </c>
@@ -27837,6 +28354,9 @@
       <c r="I514" t="s">
         <v>1</v>
       </c>
+      <c r="J514">
+        <v>2</v>
+      </c>
       <c r="K514" t="s">
         <v>71</v>
       </c>
@@ -27887,6 +28407,9 @@
       <c r="I515" t="s">
         <v>47</v>
       </c>
+      <c r="J515">
+        <v>4</v>
+      </c>
       <c r="K515" t="s">
         <v>71</v>
       </c>
@@ -27937,6 +28460,9 @@
       <c r="I516" t="s">
         <v>23</v>
       </c>
+      <c r="J516">
+        <v>1</v>
+      </c>
       <c r="K516" t="s">
         <v>71</v>
       </c>
@@ -27986,6 +28512,9 @@
       </c>
       <c r="I517" t="s">
         <v>6</v>
+      </c>
+      <c r="J517">
+        <v>2</v>
       </c>
       <c r="K517" t="s">
         <v>71</v>
@@ -28037,6 +28566,9 @@
       <c r="I518" t="s">
         <v>15</v>
       </c>
+      <c r="J518">
+        <v>-5</v>
+      </c>
       <c r="K518" t="s">
         <v>71</v>
       </c>
@@ -28087,6 +28619,9 @@
       <c r="I519" t="s">
         <v>9</v>
       </c>
+      <c r="J519">
+        <v>-1</v>
+      </c>
       <c r="K519" t="s">
         <v>71</v>
       </c>
@@ -28137,6 +28672,9 @@
       <c r="I520" t="s">
         <v>17</v>
       </c>
+      <c r="J520">
+        <v>1</v>
+      </c>
       <c r="K520" t="s">
         <v>71</v>
       </c>
@@ -28187,6 +28725,9 @@
       <c r="I521" t="s">
         <v>6</v>
       </c>
+      <c r="J521">
+        <v>2</v>
+      </c>
       <c r="K521" t="s">
         <v>71</v>
       </c>
@@ -28237,6 +28778,9 @@
       <c r="I522" t="s">
         <v>48</v>
       </c>
+      <c r="J522">
+        <v>4</v>
+      </c>
       <c r="K522" t="s">
         <v>71</v>
       </c>
@@ -28287,6 +28831,9 @@
       <c r="I523" t="s">
         <v>27</v>
       </c>
+      <c r="J523">
+        <v>1</v>
+      </c>
       <c r="K523" t="s">
         <v>71</v>
       </c>
@@ -28337,6 +28884,9 @@
       <c r="I524" t="s">
         <v>52</v>
       </c>
+      <c r="J524">
+        <v>2</v>
+      </c>
       <c r="K524" t="s">
         <v>71</v>
       </c>
@@ -28387,6 +28937,9 @@
       <c r="I525" t="s">
         <v>40</v>
       </c>
+      <c r="J525">
+        <v>5</v>
+      </c>
       <c r="K525" t="s">
         <v>71</v>
       </c>
@@ -28437,6 +28990,9 @@
       <c r="I526" t="s">
         <v>4</v>
       </c>
+      <c r="J526">
+        <v>1</v>
+      </c>
       <c r="K526" t="s">
         <v>71</v>
       </c>
@@ -28487,6 +29043,9 @@
       <c r="I527" t="s">
         <v>22</v>
       </c>
+      <c r="J527">
+        <v>2</v>
+      </c>
       <c r="K527" t="s">
         <v>71</v>
       </c>
@@ -28537,6 +29096,9 @@
       <c r="I528" t="s">
         <v>13</v>
       </c>
+      <c r="J528">
+        <v>4</v>
+      </c>
       <c r="K528" t="s">
         <v>71</v>
       </c>
@@ -28587,6 +29149,9 @@
       <c r="I529" t="s">
         <v>1</v>
       </c>
+      <c r="J529">
+        <v>1</v>
+      </c>
       <c r="K529" t="s">
         <v>71</v>
       </c>
@@ -28636,6 +29201,9 @@
       </c>
       <c r="I530" t="s">
         <v>10</v>
+      </c>
+      <c r="J530">
+        <v>2</v>
       </c>
       <c r="K530" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Up to measure 40.5 fingering
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -328,8 +328,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="247">
+  <cellStyleXfs count="291">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -581,7 +625,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="247">
+  <cellStyles count="291">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -705,6 +749,28 @@
     <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="250" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="252" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="254" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="256" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="258" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="260" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="262" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="264" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="266" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="268" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="270" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="272" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="274" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="276" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="278" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="280" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="282" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="284" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="286" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="288" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="290" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -828,6 +894,28 @@
     <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="249" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="251" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="253" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="255" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="257" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="259" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="261" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="263" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="265" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="267" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="269" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="271" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="273" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="275" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="277" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="279" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="281" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="283" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="285" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="287" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="289" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1160,8 +1248,8 @@
   <dimension ref="A1:Q1181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A502" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J529" sqref="J529"/>
+      <pane ySplit="1" topLeftCell="A633" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J647" sqref="J647"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -29255,6 +29343,9 @@
       <c r="I531" t="s">
         <v>1</v>
       </c>
+      <c r="J531">
+        <v>-5</v>
+      </c>
       <c r="K531" t="s">
         <v>71</v>
       </c>
@@ -29305,6 +29396,9 @@
       <c r="I532" t="s">
         <v>11</v>
       </c>
+      <c r="J532">
+        <v>-1</v>
+      </c>
       <c r="K532" t="s">
         <v>71</v>
       </c>
@@ -29355,6 +29449,9 @@
       <c r="I533" t="s">
         <v>21</v>
       </c>
+      <c r="J533">
+        <v>1</v>
+      </c>
       <c r="K533" t="s">
         <v>71</v>
       </c>
@@ -29405,6 +29502,9 @@
       <c r="I534" t="s">
         <v>18</v>
       </c>
+      <c r="J534">
+        <v>3</v>
+      </c>
       <c r="K534" t="s">
         <v>71</v>
       </c>
@@ -29455,6 +29555,9 @@
       <c r="I535" t="s">
         <v>0</v>
       </c>
+      <c r="J535">
+        <v>2</v>
+      </c>
       <c r="K535" t="s">
         <v>71</v>
       </c>
@@ -29505,6 +29608,9 @@
       <c r="I536" t="s">
         <v>47</v>
       </c>
+      <c r="J536">
+        <v>5</v>
+      </c>
       <c r="K536" t="s">
         <v>71</v>
       </c>
@@ -29555,6 +29661,9 @@
       <c r="I537" t="s">
         <v>27</v>
       </c>
+      <c r="J537">
+        <v>1</v>
+      </c>
       <c r="K537" t="s">
         <v>71</v>
       </c>
@@ -29605,6 +29714,9 @@
       <c r="I538" t="s">
         <v>52</v>
       </c>
+      <c r="J538">
+        <v>3</v>
+      </c>
       <c r="K538" t="s">
         <v>71</v>
       </c>
@@ -29655,6 +29767,9 @@
       <c r="I539" t="s">
         <v>19</v>
       </c>
+      <c r="J539">
+        <v>2</v>
+      </c>
       <c r="K539" t="s">
         <v>71</v>
       </c>
@@ -29705,6 +29820,9 @@
       <c r="I540" t="s">
         <v>53</v>
       </c>
+      <c r="J540">
+        <v>5</v>
+      </c>
       <c r="K540" t="s">
         <v>71</v>
       </c>
@@ -29755,6 +29873,9 @@
       <c r="I541" t="s">
         <v>42</v>
       </c>
+      <c r="J541">
+        <v>1</v>
+      </c>
       <c r="K541" t="s">
         <v>71</v>
       </c>
@@ -29805,6 +29926,9 @@
       <c r="I542" t="s">
         <v>2</v>
       </c>
+      <c r="J542">
+        <v>3</v>
+      </c>
       <c r="K542" t="s">
         <v>71</v>
       </c>
@@ -29855,6 +29979,9 @@
       <c r="I543" t="s">
         <v>53</v>
       </c>
+      <c r="J543">
+        <v>2</v>
+      </c>
       <c r="K543" t="s">
         <v>71</v>
       </c>
@@ -29904,6 +30031,9 @@
       </c>
       <c r="I544" t="s">
         <v>19</v>
+      </c>
+      <c r="J544">
+        <v>5</v>
       </c>
       <c r="K544" t="s">
         <v>71</v>
@@ -29955,6 +30085,9 @@
       <c r="I545" t="s">
         <v>24</v>
       </c>
+      <c r="J545">
+        <v>-5</v>
+      </c>
       <c r="K545" t="s">
         <v>71</v>
       </c>
@@ -30005,6 +30138,9 @@
       <c r="I546" t="s">
         <v>12</v>
       </c>
+      <c r="J546">
+        <v>-1</v>
+      </c>
       <c r="K546" t="s">
         <v>71</v>
       </c>
@@ -30055,6 +30191,9 @@
       <c r="I547" t="s">
         <v>42</v>
       </c>
+      <c r="J547">
+        <v>1</v>
+      </c>
       <c r="K547" t="s">
         <v>71</v>
       </c>
@@ -30105,6 +30244,9 @@
       <c r="I548" t="s">
         <v>17</v>
       </c>
+      <c r="J548">
+        <v>4</v>
+      </c>
       <c r="K548" t="s">
         <v>71</v>
       </c>
@@ -30155,6 +30297,9 @@
       <c r="I549" t="s">
         <v>44</v>
       </c>
+      <c r="J549">
+        <v>2</v>
+      </c>
       <c r="K549" t="s">
         <v>71</v>
       </c>
@@ -30205,6 +30350,9 @@
       <c r="I550" t="s">
         <v>2</v>
       </c>
+      <c r="J550">
+        <v>5</v>
+      </c>
       <c r="K550" t="s">
         <v>71</v>
       </c>
@@ -30255,6 +30403,9 @@
       <c r="I551" t="s">
         <v>22</v>
       </c>
+      <c r="J551">
+        <v>1</v>
+      </c>
       <c r="K551" t="s">
         <v>71</v>
       </c>
@@ -30305,6 +30456,9 @@
       <c r="I552" t="s">
         <v>25</v>
       </c>
+      <c r="J552">
+        <v>3</v>
+      </c>
       <c r="K552" t="s">
         <v>71</v>
       </c>
@@ -30355,6 +30509,9 @@
       <c r="I553" t="s">
         <v>3</v>
       </c>
+      <c r="J553">
+        <v>2</v>
+      </c>
       <c r="K553" t="s">
         <v>71</v>
       </c>
@@ -30405,6 +30562,9 @@
       <c r="I554" t="s">
         <v>31</v>
       </c>
+      <c r="J554">
+        <v>5</v>
+      </c>
       <c r="K554" t="s">
         <v>71</v>
       </c>
@@ -30455,6 +30615,9 @@
       <c r="I555" t="s">
         <v>3</v>
       </c>
+      <c r="J555">
+        <v>1</v>
+      </c>
       <c r="K555" t="s">
         <v>71</v>
       </c>
@@ -30505,6 +30668,9 @@
       <c r="I556" t="s">
         <v>19</v>
       </c>
+      <c r="J556">
+        <v>4</v>
+      </c>
       <c r="K556" t="s">
         <v>71</v>
       </c>
@@ -30555,6 +30721,9 @@
       <c r="I557" t="s">
         <v>29</v>
       </c>
+      <c r="J557">
+        <v>2</v>
+      </c>
       <c r="K557" t="s">
         <v>71</v>
       </c>
@@ -30604,6 +30773,9 @@
       </c>
       <c r="I558" t="s">
         <v>12</v>
+      </c>
+      <c r="J558">
+        <v>1</v>
       </c>
       <c r="K558" t="s">
         <v>71</v>
@@ -30655,6 +30827,9 @@
       <c r="I559" t="s">
         <v>44</v>
       </c>
+      <c r="J559">
+        <v>-5</v>
+      </c>
       <c r="K559" t="s">
         <v>71</v>
       </c>
@@ -30705,6 +30880,9 @@
       <c r="I560" t="s">
         <v>16</v>
       </c>
+      <c r="J560">
+        <v>-1</v>
+      </c>
       <c r="K560" t="s">
         <v>71</v>
       </c>
@@ -30755,6 +30933,9 @@
       <c r="I561" t="s">
         <v>21</v>
       </c>
+      <c r="J561">
+        <v>1</v>
+      </c>
       <c r="K561" t="s">
         <v>71</v>
       </c>
@@ -30805,6 +30986,9 @@
       <c r="I562" t="s">
         <v>33</v>
       </c>
+      <c r="J562">
+        <v>3</v>
+      </c>
       <c r="K562" t="s">
         <v>71</v>
       </c>
@@ -30855,6 +31039,9 @@
       <c r="I563" t="s">
         <v>49</v>
       </c>
+      <c r="J563">
+        <v>2</v>
+      </c>
       <c r="K563" t="s">
         <v>71</v>
       </c>
@@ -30905,6 +31092,9 @@
       <c r="I564" t="s">
         <v>2</v>
       </c>
+      <c r="J564">
+        <v>5</v>
+      </c>
       <c r="K564" t="s">
         <v>71</v>
       </c>
@@ -30955,6 +31145,9 @@
       <c r="I565" t="s">
         <v>14</v>
       </c>
+      <c r="J565">
+        <v>1</v>
+      </c>
       <c r="K565" t="s">
         <v>71</v>
       </c>
@@ -31005,6 +31198,9 @@
       <c r="I566" t="s">
         <v>2</v>
       </c>
+      <c r="J566">
+        <v>3</v>
+      </c>
       <c r="K566" t="s">
         <v>71</v>
       </c>
@@ -31055,6 +31251,9 @@
       <c r="I567" t="s">
         <v>27</v>
       </c>
+      <c r="J567">
+        <v>2</v>
+      </c>
       <c r="K567" t="s">
         <v>71</v>
       </c>
@@ -31105,6 +31304,9 @@
       <c r="I568" t="s">
         <v>26</v>
       </c>
+      <c r="J568">
+        <v>5</v>
+      </c>
       <c r="K568" t="s">
         <v>71</v>
       </c>
@@ -31155,6 +31357,9 @@
       <c r="I569" t="s">
         <v>15</v>
       </c>
+      <c r="J569">
+        <v>1</v>
+      </c>
       <c r="K569" t="s">
         <v>71</v>
       </c>
@@ -31205,6 +31410,9 @@
       <c r="I570" t="s">
         <v>31</v>
       </c>
+      <c r="J570">
+        <v>3</v>
+      </c>
       <c r="K570" t="s">
         <v>71</v>
       </c>
@@ -31255,6 +31463,9 @@
       <c r="I571" t="s">
         <v>44</v>
       </c>
+      <c r="J571">
+        <v>2</v>
+      </c>
       <c r="K571" t="s">
         <v>71</v>
       </c>
@@ -31304,6 +31515,9 @@
       </c>
       <c r="I572" t="s">
         <v>12</v>
+      </c>
+      <c r="J572">
+        <v>5</v>
       </c>
       <c r="K572" t="s">
         <v>71</v>
@@ -31355,6 +31569,9 @@
       <c r="I573" t="s">
         <v>10</v>
       </c>
+      <c r="J573">
+        <v>-5</v>
+      </c>
       <c r="K573" t="s">
         <v>71</v>
       </c>
@@ -31405,6 +31622,9 @@
       <c r="I574" t="s">
         <v>17</v>
       </c>
+      <c r="J574">
+        <v>-1</v>
+      </c>
       <c r="K574" t="s">
         <v>71</v>
       </c>
@@ -31455,6 +31675,9 @@
       <c r="I575" t="s">
         <v>1</v>
       </c>
+      <c r="J575">
+        <v>1</v>
+      </c>
       <c r="K575" t="s">
         <v>71</v>
       </c>
@@ -31505,6 +31728,9 @@
       <c r="I576" t="s">
         <v>20</v>
       </c>
+      <c r="J576">
+        <v>3</v>
+      </c>
       <c r="K576" t="s">
         <v>71</v>
       </c>
@@ -31555,6 +31781,9 @@
       <c r="I577" t="s">
         <v>21</v>
       </c>
+      <c r="J577">
+        <v>2</v>
+      </c>
       <c r="K577" t="s">
         <v>71</v>
       </c>
@@ -31605,6 +31834,9 @@
       <c r="I578" t="s">
         <v>32</v>
       </c>
+      <c r="J578">
+        <v>5</v>
+      </c>
       <c r="K578" t="s">
         <v>71</v>
       </c>
@@ -31655,6 +31887,9 @@
       <c r="I579" t="s">
         <v>12</v>
       </c>
+      <c r="J579">
+        <v>1</v>
+      </c>
       <c r="K579" t="s">
         <v>71</v>
       </c>
@@ -31705,6 +31940,9 @@
       <c r="I580" t="s">
         <v>42</v>
       </c>
+      <c r="J580">
+        <v>3</v>
+      </c>
       <c r="K580" t="s">
         <v>71</v>
       </c>
@@ -31755,6 +31993,9 @@
       <c r="I581" t="s">
         <v>42</v>
       </c>
+      <c r="J581">
+        <v>2</v>
+      </c>
       <c r="K581" t="s">
         <v>71</v>
       </c>
@@ -31805,6 +32046,9 @@
       <c r="I582" t="s">
         <v>8</v>
       </c>
+      <c r="J582">
+        <v>5</v>
+      </c>
       <c r="K582" t="s">
         <v>71</v>
       </c>
@@ -31855,6 +32099,9 @@
       <c r="I583" t="s">
         <v>21</v>
       </c>
+      <c r="J583">
+        <v>1</v>
+      </c>
       <c r="K583" t="s">
         <v>71</v>
       </c>
@@ -31905,6 +32152,9 @@
       <c r="I584" t="s">
         <v>40</v>
       </c>
+      <c r="J584">
+        <v>3</v>
+      </c>
       <c r="K584" t="s">
         <v>71</v>
       </c>
@@ -31955,6 +32205,9 @@
       <c r="I585" t="s">
         <v>44</v>
       </c>
+      <c r="J585">
+        <v>2</v>
+      </c>
       <c r="K585" t="s">
         <v>71</v>
       </c>
@@ -32004,6 +32257,9 @@
       </c>
       <c r="I586" t="s">
         <v>42</v>
+      </c>
+      <c r="J586">
+        <v>5</v>
       </c>
       <c r="K586" t="s">
         <v>71</v>
@@ -32055,6 +32311,9 @@
       <c r="I587" t="s">
         <v>19</v>
       </c>
+      <c r="J587">
+        <v>5</v>
+      </c>
       <c r="K587" t="s">
         <v>71</v>
       </c>
@@ -32105,6 +32364,9 @@
       <c r="I588" t="s">
         <v>10</v>
       </c>
+      <c r="J588">
+        <v>2</v>
+      </c>
       <c r="K588" t="s">
         <v>71</v>
       </c>
@@ -32155,6 +32417,9 @@
       <c r="I589" t="s">
         <v>23</v>
       </c>
+      <c r="J589">
+        <v>3</v>
+      </c>
       <c r="K589" t="s">
         <v>71</v>
       </c>
@@ -32205,6 +32470,9 @@
       <c r="I590" t="s">
         <v>13</v>
       </c>
+      <c r="J590">
+        <v>1</v>
+      </c>
       <c r="K590" t="s">
         <v>71</v>
       </c>
@@ -32255,6 +32523,9 @@
       <c r="I591" t="s">
         <v>22</v>
       </c>
+      <c r="J591">
+        <v>5</v>
+      </c>
       <c r="K591" t="s">
         <v>71</v>
       </c>
@@ -32305,6 +32576,9 @@
       <c r="I592" t="s">
         <v>24</v>
       </c>
+      <c r="J592">
+        <v>2</v>
+      </c>
       <c r="K592" t="s">
         <v>71</v>
       </c>
@@ -32355,6 +32629,9 @@
       <c r="I593" t="s">
         <v>41</v>
       </c>
+      <c r="J593">
+        <v>3</v>
+      </c>
       <c r="K593" t="s">
         <v>71</v>
       </c>
@@ -32405,6 +32682,9 @@
       <c r="I594" t="s">
         <v>17</v>
       </c>
+      <c r="J594">
+        <v>1</v>
+      </c>
       <c r="K594" t="s">
         <v>71</v>
       </c>
@@ -32455,6 +32735,9 @@
       <c r="I595" t="s">
         <v>12</v>
       </c>
+      <c r="J595">
+        <v>5</v>
+      </c>
       <c r="K595" t="s">
         <v>71</v>
       </c>
@@ -32505,6 +32788,9 @@
       <c r="I596" t="s">
         <v>27</v>
       </c>
+      <c r="J596">
+        <v>2</v>
+      </c>
       <c r="K596" t="s">
         <v>71</v>
       </c>
@@ -32555,6 +32841,9 @@
       <c r="I597" t="s">
         <v>29</v>
       </c>
+      <c r="J597">
+        <v>3</v>
+      </c>
       <c r="K597" t="s">
         <v>71</v>
       </c>
@@ -32604,6 +32893,9 @@
       </c>
       <c r="I598" t="s">
         <v>18</v>
+      </c>
+      <c r="J598">
+        <v>1</v>
       </c>
       <c r="K598" t="s">
         <v>71</v>
@@ -32655,6 +32947,9 @@
       <c r="I599" t="s">
         <v>0</v>
       </c>
+      <c r="J599">
+        <v>5</v>
+      </c>
       <c r="K599" t="s">
         <v>71</v>
       </c>
@@ -32705,6 +33000,9 @@
       <c r="I600" t="s">
         <v>22</v>
       </c>
+      <c r="J600">
+        <v>2</v>
+      </c>
       <c r="K600" t="s">
         <v>71</v>
       </c>
@@ -32755,6 +33053,9 @@
       <c r="I601" t="s">
         <v>11</v>
       </c>
+      <c r="J601">
+        <v>3</v>
+      </c>
       <c r="K601" t="s">
         <v>71</v>
       </c>
@@ -32805,6 +33106,9 @@
       <c r="I602" t="s">
         <v>42</v>
       </c>
+      <c r="J602">
+        <v>1</v>
+      </c>
       <c r="K602" t="s">
         <v>71</v>
       </c>
@@ -32855,6 +33159,9 @@
       <c r="I603" t="s">
         <v>12</v>
       </c>
+      <c r="J603">
+        <v>5</v>
+      </c>
       <c r="K603" t="s">
         <v>71</v>
       </c>
@@ -32905,6 +33212,9 @@
       <c r="I604" t="s">
         <v>8</v>
       </c>
+      <c r="J604">
+        <v>2</v>
+      </c>
       <c r="K604" t="s">
         <v>71</v>
       </c>
@@ -32955,6 +33265,9 @@
       <c r="I605" t="s">
         <v>6</v>
       </c>
+      <c r="J605">
+        <v>3</v>
+      </c>
       <c r="K605" t="s">
         <v>71</v>
       </c>
@@ -33005,6 +33318,9 @@
       <c r="I606" t="s">
         <v>46</v>
       </c>
+      <c r="J606">
+        <v>1</v>
+      </c>
       <c r="K606" t="s">
         <v>71</v>
       </c>
@@ -33055,6 +33371,9 @@
       <c r="I607" t="s">
         <v>3</v>
       </c>
+      <c r="J607">
+        <v>2</v>
+      </c>
       <c r="K607" t="s">
         <v>71</v>
       </c>
@@ -33105,6 +33424,9 @@
       <c r="I608" t="s">
         <v>5</v>
       </c>
+      <c r="J608">
+        <v>1</v>
+      </c>
       <c r="K608" t="s">
         <v>71</v>
       </c>
@@ -33155,6 +33477,9 @@
       <c r="I609" t="s">
         <v>44</v>
       </c>
+      <c r="J609">
+        <v>2</v>
+      </c>
       <c r="K609" t="s">
         <v>71</v>
       </c>
@@ -33204,6 +33529,9 @@
       </c>
       <c r="I610" t="s">
         <v>14</v>
+      </c>
+      <c r="J610">
+        <v>3</v>
       </c>
       <c r="K610" t="s">
         <v>71</v>
@@ -33255,6 +33583,9 @@
       <c r="I611" t="s">
         <v>14</v>
       </c>
+      <c r="J611">
+        <v>-5</v>
+      </c>
       <c r="K611" t="s">
         <v>71</v>
       </c>
@@ -33305,6 +33636,9 @@
       <c r="I612" t="s">
         <v>10</v>
       </c>
+      <c r="J612">
+        <v>-1</v>
+      </c>
       <c r="K612" t="s">
         <v>71</v>
       </c>
@@ -33355,6 +33689,9 @@
       <c r="I613" t="s">
         <v>27</v>
       </c>
+      <c r="J613">
+        <v>1</v>
+      </c>
       <c r="K613" t="s">
         <v>71</v>
       </c>
@@ -33405,6 +33742,9 @@
       <c r="I614" t="s">
         <v>14</v>
       </c>
+      <c r="J614">
+        <v>2</v>
+      </c>
       <c r="K614" t="s">
         <v>71</v>
       </c>
@@ -33455,6 +33795,9 @@
       <c r="I615" t="s">
         <v>27</v>
       </c>
+      <c r="J615">
+        <v>3</v>
+      </c>
       <c r="K615" t="s">
         <v>71</v>
       </c>
@@ -33505,6 +33848,9 @@
       <c r="I616" t="s">
         <v>25</v>
       </c>
+      <c r="J616">
+        <v>4</v>
+      </c>
       <c r="K616" t="s">
         <v>71</v>
       </c>
@@ -33555,6 +33901,9 @@
       <c r="I617" t="s">
         <v>9</v>
       </c>
+      <c r="J617">
+        <v>3</v>
+      </c>
       <c r="K617" t="s">
         <v>71</v>
       </c>
@@ -33605,6 +33954,9 @@
       <c r="I618" t="s">
         <v>42</v>
       </c>
+      <c r="J618">
+        <v>2</v>
+      </c>
       <c r="K618" t="s">
         <v>71</v>
       </c>
@@ -33655,6 +34007,9 @@
       <c r="I619" t="s">
         <v>50</v>
       </c>
+      <c r="J619">
+        <v>1</v>
+      </c>
       <c r="K619" t="s">
         <v>71</v>
       </c>
@@ -33705,6 +34060,9 @@
       <c r="I620" t="s">
         <v>9</v>
       </c>
+      <c r="J620">
+        <v>2</v>
+      </c>
       <c r="K620" t="s">
         <v>71</v>
       </c>
@@ -33755,6 +34113,9 @@
       <c r="I621" t="s">
         <v>44</v>
       </c>
+      <c r="J621">
+        <v>4</v>
+      </c>
       <c r="K621" t="s">
         <v>71</v>
       </c>
@@ -33805,6 +34166,9 @@
       <c r="I622" t="s">
         <v>40</v>
       </c>
+      <c r="J622">
+        <v>1</v>
+      </c>
       <c r="K622" t="s">
         <v>71</v>
       </c>
@@ -33855,6 +34219,9 @@
       <c r="I623" t="s">
         <v>24</v>
       </c>
+      <c r="J623">
+        <v>2</v>
+      </c>
       <c r="K623" t="s">
         <v>71</v>
       </c>
@@ -33904,6 +34271,9 @@
       </c>
       <c r="I624" t="s">
         <v>10</v>
+      </c>
+      <c r="J624">
+        <v>4</v>
       </c>
       <c r="K624" t="s">
         <v>71</v>
@@ -33955,6 +34325,9 @@
       <c r="I625" t="s">
         <v>4</v>
       </c>
+      <c r="J625">
+        <v>-5</v>
+      </c>
       <c r="K625" t="s">
         <v>71</v>
       </c>
@@ -34005,6 +34378,9 @@
       <c r="I626" t="s">
         <v>10</v>
       </c>
+      <c r="J626">
+        <v>-1</v>
+      </c>
       <c r="K626" t="s">
         <v>71</v>
       </c>
@@ -34055,6 +34431,9 @@
       <c r="I627" t="s">
         <v>33</v>
       </c>
+      <c r="J627">
+        <v>1</v>
+      </c>
       <c r="K627" t="s">
         <v>71</v>
       </c>
@@ -34105,6 +34484,9 @@
       <c r="I628" t="s">
         <v>17</v>
       </c>
+      <c r="J628">
+        <v>2</v>
+      </c>
       <c r="K628" t="s">
         <v>71</v>
       </c>
@@ -34155,6 +34537,9 @@
       <c r="I629" t="s">
         <v>31</v>
       </c>
+      <c r="J629">
+        <v>3</v>
+      </c>
       <c r="K629" t="s">
         <v>71</v>
       </c>
@@ -34205,6 +34590,9 @@
       <c r="I630" t="s">
         <v>56</v>
       </c>
+      <c r="J630">
+        <v>4</v>
+      </c>
       <c r="K630" t="s">
         <v>71</v>
       </c>
@@ -34255,6 +34643,9 @@
       <c r="I631" t="s">
         <v>2</v>
       </c>
+      <c r="J631">
+        <v>3</v>
+      </c>
       <c r="K631" t="s">
         <v>71</v>
       </c>
@@ -34305,6 +34696,9 @@
       <c r="I632" t="s">
         <v>49</v>
       </c>
+      <c r="J632">
+        <v>2</v>
+      </c>
       <c r="K632" t="s">
         <v>71</v>
       </c>
@@ -34355,6 +34749,9 @@
       <c r="I633" t="s">
         <v>55</v>
       </c>
+      <c r="J633">
+        <v>1</v>
+      </c>
       <c r="K633" t="s">
         <v>71</v>
       </c>
@@ -34405,6 +34802,9 @@
       <c r="I634" t="s">
         <v>21</v>
       </c>
+      <c r="J634">
+        <v>2</v>
+      </c>
       <c r="K634" t="s">
         <v>71</v>
       </c>
@@ -34455,6 +34855,9 @@
       <c r="I635" t="s">
         <v>24</v>
       </c>
+      <c r="J635">
+        <v>4</v>
+      </c>
       <c r="K635" t="s">
         <v>71</v>
       </c>
@@ -34505,6 +34908,9 @@
       <c r="I636" t="s">
         <v>7</v>
       </c>
+      <c r="J636">
+        <v>1</v>
+      </c>
       <c r="K636" t="s">
         <v>71</v>
       </c>
@@ -34555,6 +34961,9 @@
       <c r="I637" t="s">
         <v>22</v>
       </c>
+      <c r="J637">
+        <v>2</v>
+      </c>
       <c r="K637" t="s">
         <v>71</v>
       </c>
@@ -34604,6 +35013,9 @@
       </c>
       <c r="I638" t="s">
         <v>20</v>
+      </c>
+      <c r="J638">
+        <v>4</v>
       </c>
       <c r="K638" t="s">
         <v>71</v>
@@ -34655,6 +35067,9 @@
       <c r="I639" t="s">
         <v>22</v>
       </c>
+      <c r="J639">
+        <v>-5</v>
+      </c>
       <c r="K639" t="s">
         <v>71</v>
       </c>
@@ -34705,6 +35120,9 @@
       <c r="I640" t="s">
         <v>18</v>
       </c>
+      <c r="J640">
+        <v>-1</v>
+      </c>
       <c r="K640" t="s">
         <v>71</v>
       </c>
@@ -34755,6 +35173,9 @@
       <c r="I641" t="s">
         <v>19</v>
       </c>
+      <c r="J641">
+        <v>1</v>
+      </c>
       <c r="K641" t="s">
         <v>71</v>
       </c>
@@ -34805,6 +35226,9 @@
       <c r="I642" t="s">
         <v>11</v>
       </c>
+      <c r="J642">
+        <v>2</v>
+      </c>
       <c r="K642" t="s">
         <v>71</v>
       </c>
@@ -34855,6 +35279,9 @@
       <c r="I643" t="s">
         <v>49</v>
       </c>
+      <c r="J643">
+        <v>3</v>
+      </c>
       <c r="K643" t="s">
         <v>71</v>
       </c>
@@ -34905,6 +35332,9 @@
       <c r="I644" t="s">
         <v>32</v>
       </c>
+      <c r="J644">
+        <v>4</v>
+      </c>
       <c r="K644" t="s">
         <v>71</v>
       </c>
@@ -34955,6 +35385,9 @@
       <c r="I645" t="s">
         <v>3</v>
       </c>
+      <c r="J645">
+        <v>3</v>
+      </c>
       <c r="K645" t="s">
         <v>71</v>
       </c>
@@ -35004,6 +35437,9 @@
       </c>
       <c r="I646" t="s">
         <v>53</v>
+      </c>
+      <c r="J646">
+        <v>2</v>
       </c>
       <c r="K646" t="s">
         <v>71</v>

</xml_diff>

<commit_message>
Add 0 for fingering so that uglifier won't complain
</commit_message>
<xml_diff>
--- a/midiParser/MoonlightSonanta.xlsx
+++ b/midiParser/MoonlightSonanta.xlsx
@@ -328,8 +328,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="303">
+  <cellStyleXfs count="305">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -637,7 +639,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="303">
+  <cellStyles count="305">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -789,6 +791,7 @@
     <cellStyle name="Followed Hyperlink" xfId="298" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="300" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="302" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="304" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -940,6 +943,7 @@
     <cellStyle name="Hyperlink" xfId="297" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="299" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="301" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="303" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1272,8 +1276,8 @@
   <dimension ref="A1:Q1180"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A473" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J499" sqref="J499"/>
+      <pane ySplit="1" topLeftCell="A1118" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="S1145" sqref="S1145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -40656,6 +40660,9 @@
       <c r="I744" t="s">
         <v>43</v>
       </c>
+      <c r="J744">
+        <v>0</v>
+      </c>
       <c r="K744" t="s">
         <v>71</v>
       </c>
@@ -40706,6 +40713,9 @@
       <c r="I745" t="s">
         <v>44</v>
       </c>
+      <c r="J745">
+        <v>0</v>
+      </c>
       <c r="K745" t="s">
         <v>71</v>
       </c>
@@ -40756,6 +40766,9 @@
       <c r="I746" t="s">
         <v>33</v>
       </c>
+      <c r="J746">
+        <v>0</v>
+      </c>
       <c r="K746" t="s">
         <v>71</v>
       </c>
@@ -40806,6 +40819,9 @@
       <c r="I747" t="s">
         <v>15</v>
       </c>
+      <c r="J747">
+        <v>0</v>
+      </c>
       <c r="K747" t="s">
         <v>71</v>
       </c>
@@ -40856,6 +40872,9 @@
       <c r="I748" t="s">
         <v>33</v>
       </c>
+      <c r="J748">
+        <v>0</v>
+      </c>
       <c r="K748" t="s">
         <v>71</v>
       </c>
@@ -40906,6 +40925,9 @@
       <c r="I749" t="s">
         <v>14</v>
       </c>
+      <c r="J749">
+        <v>0</v>
+      </c>
       <c r="K749" t="s">
         <v>71</v>
       </c>
@@ -40956,6 +40978,9 @@
       <c r="I750" t="s">
         <v>14</v>
       </c>
+      <c r="J750">
+        <v>0</v>
+      </c>
       <c r="K750" t="s">
         <v>71</v>
       </c>
@@ -41006,6 +41031,9 @@
       <c r="I751" t="s">
         <v>33</v>
       </c>
+      <c r="J751">
+        <v>0</v>
+      </c>
       <c r="K751" t="s">
         <v>71</v>
       </c>
@@ -41056,6 +41084,9 @@
       <c r="I752" t="s">
         <v>10</v>
       </c>
+      <c r="J752">
+        <v>0</v>
+      </c>
       <c r="K752" t="s">
         <v>71</v>
       </c>
@@ -41106,6 +41137,9 @@
       <c r="I753" t="s">
         <v>10</v>
       </c>
+      <c r="J753">
+        <v>0</v>
+      </c>
       <c r="K753" t="s">
         <v>71</v>
       </c>
@@ -41156,6 +41190,9 @@
       <c r="I754" t="s">
         <v>49</v>
       </c>
+      <c r="J754">
+        <v>0</v>
+      </c>
       <c r="K754" t="s">
         <v>71</v>
       </c>
@@ -41206,6 +41243,9 @@
       <c r="I755" t="s">
         <v>31</v>
       </c>
+      <c r="J755">
+        <v>0</v>
+      </c>
       <c r="K755" t="s">
         <v>71</v>
       </c>
@@ -41256,6 +41296,9 @@
       <c r="I756" t="s">
         <v>17</v>
       </c>
+      <c r="J756">
+        <v>0</v>
+      </c>
       <c r="K756" t="s">
         <v>71</v>
       </c>
@@ -41306,6 +41349,9 @@
       <c r="I757" t="s">
         <v>22</v>
       </c>
+      <c r="J757">
+        <v>0</v>
+      </c>
       <c r="K757" t="s">
         <v>71</v>
       </c>
@@ -41355,6 +41401,9 @@
       </c>
       <c r="I758" t="s">
         <v>24</v>
+      </c>
+      <c r="J758">
+        <v>0</v>
       </c>
       <c r="K758" t="s">
         <v>71</v>
@@ -41406,6 +41455,9 @@
       <c r="I759" t="s">
         <v>12</v>
       </c>
+      <c r="J759">
+        <v>0</v>
+      </c>
       <c r="K759" t="s">
         <v>71</v>
       </c>
@@ -41456,6 +41508,9 @@
       <c r="I760" t="s">
         <v>44</v>
       </c>
+      <c r="J760">
+        <v>0</v>
+      </c>
       <c r="K760" t="s">
         <v>71</v>
       </c>
@@ -41506,6 +41561,9 @@
       <c r="I761" t="s">
         <v>44</v>
       </c>
+      <c r="J761">
+        <v>0</v>
+      </c>
       <c r="K761" t="s">
         <v>71</v>
       </c>
@@ -41556,6 +41614,9 @@
       <c r="I762" t="s">
         <v>19</v>
       </c>
+      <c r="J762">
+        <v>0</v>
+      </c>
       <c r="K762" t="s">
         <v>71</v>
       </c>
@@ -41606,6 +41667,9 @@
       <c r="I763" t="s">
         <v>16</v>
       </c>
+      <c r="J763">
+        <v>0</v>
+      </c>
       <c r="K763" t="s">
         <v>71</v>
       </c>
@@ -41656,6 +41720,9 @@
       <c r="I764" t="s">
         <v>37</v>
       </c>
+      <c r="J764">
+        <v>0</v>
+      </c>
       <c r="K764" t="s">
         <v>71</v>
       </c>
@@ -41706,6 +41773,9 @@
       <c r="I765" t="s">
         <v>15</v>
       </c>
+      <c r="J765">
+        <v>0</v>
+      </c>
       <c r="K765" t="s">
         <v>71</v>
       </c>
@@ -41756,6 +41826,9 @@
       <c r="I766" t="s">
         <v>36</v>
       </c>
+      <c r="J766">
+        <v>0</v>
+      </c>
       <c r="K766" t="s">
         <v>71</v>
       </c>
@@ -41806,6 +41879,9 @@
       <c r="I767" t="s">
         <v>29</v>
       </c>
+      <c r="J767">
+        <v>0</v>
+      </c>
       <c r="K767" t="s">
         <v>71</v>
       </c>
@@ -41856,6 +41932,9 @@
       <c r="I768" t="s">
         <v>12</v>
       </c>
+      <c r="J768">
+        <v>0</v>
+      </c>
       <c r="K768" t="s">
         <v>71</v>
       </c>
@@ -41906,6 +41985,9 @@
       <c r="I769" t="s">
         <v>11</v>
       </c>
+      <c r="J769">
+        <v>0</v>
+      </c>
       <c r="K769" t="s">
         <v>71</v>
       </c>
@@ -41956,6 +42038,9 @@
       <c r="I770" t="s">
         <v>10</v>
       </c>
+      <c r="J770">
+        <v>0</v>
+      </c>
       <c r="K770" t="s">
         <v>71</v>
       </c>
@@ -42006,6 +42091,9 @@
       <c r="I771" t="s">
         <v>27</v>
       </c>
+      <c r="J771">
+        <v>0</v>
+      </c>
       <c r="K771" t="s">
         <v>71</v>
       </c>
@@ -42056,6 +42144,9 @@
       <c r="I772" t="s">
         <v>40</v>
       </c>
+      <c r="J772">
+        <v>0</v>
+      </c>
       <c r="K772" t="s">
         <v>71</v>
       </c>
@@ -42106,6 +42197,9 @@
       <c r="I773" t="s">
         <v>23</v>
       </c>
+      <c r="J773">
+        <v>0</v>
+      </c>
       <c r="K773" t="s">
         <v>71</v>
       </c>
@@ -42156,6 +42250,9 @@
       <c r="I774" t="s">
         <v>12</v>
       </c>
+      <c r="J774">
+        <v>0</v>
+      </c>
       <c r="K774" t="s">
         <v>71</v>
       </c>
@@ -42204,6 +42301,9 @@
         <v>50</v>
       </c>
       <c r="I775" t="s">
+        <v>0</v>
+      </c>
+      <c r="J775">
         <v>0</v>
       </c>
       <c r="K775" t="s">
@@ -42256,6 +42356,9 @@
       <c r="I776" t="s">
         <v>15</v>
       </c>
+      <c r="J776">
+        <v>0</v>
+      </c>
       <c r="K776" t="s">
         <v>71</v>
       </c>
@@ -42306,6 +42409,9 @@
       <c r="I777" t="s">
         <v>24</v>
       </c>
+      <c r="J777">
+        <v>0</v>
+      </c>
       <c r="K777" t="s">
         <v>71</v>
       </c>
@@ -42356,6 +42462,9 @@
       <c r="I778" t="s">
         <v>22</v>
       </c>
+      <c r="J778">
+        <v>0</v>
+      </c>
       <c r="K778" t="s">
         <v>71</v>
       </c>
@@ -42406,6 +42515,9 @@
       <c r="I779" t="s">
         <v>2</v>
       </c>
+      <c r="J779">
+        <v>0</v>
+      </c>
       <c r="K779" t="s">
         <v>71</v>
       </c>
@@ -42456,6 +42568,9 @@
       <c r="I780" t="s">
         <v>17</v>
       </c>
+      <c r="J780">
+        <v>0</v>
+      </c>
       <c r="K780" t="s">
         <v>71</v>
       </c>
@@ -42506,6 +42621,9 @@
       <c r="I781" t="s">
         <v>24</v>
       </c>
+      <c r="J781">
+        <v>0</v>
+      </c>
       <c r="K781" t="s">
         <v>71</v>
       </c>
@@ -42556,6 +42674,9 @@
       <c r="I782" t="s">
         <v>13</v>
       </c>
+      <c r="J782">
+        <v>0</v>
+      </c>
       <c r="K782" t="s">
         <v>71</v>
       </c>
@@ -42606,6 +42727,9 @@
       <c r="I783" t="s">
         <v>44</v>
       </c>
+      <c r="J783">
+        <v>0</v>
+      </c>
       <c r="K783" t="s">
         <v>71</v>
       </c>
@@ -42656,6 +42780,9 @@
       <c r="I784" t="s">
         <v>16</v>
       </c>
+      <c r="J784">
+        <v>0</v>
+      </c>
       <c r="K784" t="s">
         <v>71</v>
       </c>
@@ -42706,6 +42833,9 @@
       <c r="I785" t="s">
         <v>52</v>
       </c>
+      <c r="J785">
+        <v>0</v>
+      </c>
       <c r="K785" t="s">
         <v>71</v>
       </c>
@@ -42756,6 +42886,9 @@
       <c r="I786" t="s">
         <v>19</v>
       </c>
+      <c r="J786">
+        <v>0</v>
+      </c>
       <c r="K786" t="s">
         <v>71</v>
       </c>
@@ -42806,6 +42939,9 @@
       <c r="I787" t="s">
         <v>59</v>
       </c>
+      <c r="J787">
+        <v>0</v>
+      </c>
       <c r="K787" t="s">
         <v>71</v>
       </c>
@@ -42856,6 +42992,9 @@
       <c r="I788" t="s">
         <v>63</v>
       </c>
+      <c r="J788">
+        <v>0</v>
+      </c>
       <c r="K788" t="s">
         <v>71</v>
       </c>
@@ -42906,6 +43045,9 @@
       <c r="I789" t="s">
         <v>12</v>
       </c>
+      <c r="J789">
+        <v>0</v>
+      </c>
       <c r="K789" t="s">
         <v>71</v>
       </c>
@@ -42956,6 +43098,9 @@
       <c r="I790" t="s">
         <v>47</v>
       </c>
+      <c r="J790">
+        <v>0</v>
+      </c>
       <c r="K790" t="s">
         <v>71</v>
       </c>
@@ -43006,6 +43151,9 @@
       <c r="I791" t="s">
         <v>19</v>
       </c>
+      <c r="J791">
+        <v>0</v>
+      </c>
       <c r="K791" t="s">
         <v>71</v>
       </c>
@@ -43056,6 +43204,9 @@
       <c r="I792" t="s">
         <v>54</v>
       </c>
+      <c r="J792">
+        <v>0</v>
+      </c>
       <c r="K792" t="s">
         <v>71</v>
       </c>
@@ -43106,6 +43257,9 @@
       <c r="I793" t="s">
         <v>0</v>
       </c>
+      <c r="J793">
+        <v>0</v>
+      </c>
       <c r="K793" t="s">
         <v>71</v>
       </c>
@@ -43156,6 +43310,9 @@
       <c r="I794" t="s">
         <v>64</v>
       </c>
+      <c r="J794">
+        <v>0</v>
+      </c>
       <c r="K794" t="s">
         <v>71</v>
       </c>
@@ -43206,6 +43363,9 @@
       <c r="I795" t="s">
         <v>33</v>
       </c>
+      <c r="J795">
+        <v>0</v>
+      </c>
       <c r="K795" t="s">
         <v>71</v>
       </c>
@@ -43255,6 +43415,9 @@
       </c>
       <c r="I796" t="s">
         <v>41</v>
+      </c>
+      <c r="J796">
+        <v>0</v>
       </c>
       <c r="K796" t="s">
         <v>71</v>
@@ -43306,6 +43469,9 @@
       <c r="I797" t="s">
         <v>47</v>
       </c>
+      <c r="J797">
+        <v>0</v>
+      </c>
       <c r="K797" t="s">
         <v>71</v>
       </c>
@@ -43356,6 +43522,9 @@
       <c r="I798" t="s">
         <v>44</v>
       </c>
+      <c r="J798">
+        <v>0</v>
+      </c>
       <c r="K798" t="s">
         <v>71</v>
       </c>
@@ -43406,6 +43575,9 @@
       <c r="I799" t="s">
         <v>28</v>
       </c>
+      <c r="J799">
+        <v>0</v>
+      </c>
       <c r="K799" t="s">
         <v>71</v>
       </c>
@@ -43456,6 +43628,9 @@
       <c r="I800" t="s">
         <v>54</v>
       </c>
+      <c r="J800">
+        <v>0</v>
+      </c>
       <c r="K800" t="s">
         <v>71</v>
       </c>
@@ -43506,6 +43681,9 @@
       <c r="I801" t="s">
         <v>64</v>
       </c>
+      <c r="J801">
+        <v>0</v>
+      </c>
       <c r="K801" t="s">
         <v>71</v>
       </c>
@@ -43556,6 +43734,9 @@
       <c r="I802" t="s">
         <v>15</v>
       </c>
+      <c r="J802">
+        <v>0</v>
+      </c>
       <c r="K802" t="s">
         <v>71</v>
       </c>
@@ -43606,6 +43787,9 @@
       <c r="I803" t="s">
         <v>15</v>
       </c>
+      <c r="J803">
+        <v>0</v>
+      </c>
       <c r="K803" t="s">
         <v>71</v>
       </c>
@@ -43656,6 +43840,9 @@
       <c r="I804" t="s">
         <v>0</v>
       </c>
+      <c r="J804">
+        <v>0</v>
+      </c>
       <c r="K804" t="s">
         <v>71</v>
       </c>
@@ -43706,6 +43893,9 @@
       <c r="I805" t="s">
         <v>22</v>
       </c>
+      <c r="J805">
+        <v>0</v>
+      </c>
       <c r="K805" t="s">
         <v>71</v>
       </c>
@@ -43756,6 +43946,9 @@
       <c r="I806" t="s">
         <v>3</v>
       </c>
+      <c r="J806">
+        <v>0</v>
+      </c>
       <c r="K806" t="s">
         <v>71</v>
       </c>
@@ -43806,6 +43999,9 @@
       <c r="I807" t="s">
         <v>9</v>
       </c>
+      <c r="J807">
+        <v>0</v>
+      </c>
       <c r="K807" t="s">
         <v>71</v>
       </c>
@@ -43856,6 +44052,9 @@
       <c r="I808" t="s">
         <v>8</v>
       </c>
+      <c r="J808">
+        <v>0</v>
+      </c>
       <c r="K808" t="s">
         <v>71</v>
       </c>
@@ -43906,6 +44105,9 @@
       <c r="I809" t="s">
         <v>24</v>
       </c>
+      <c r="J809">
+        <v>0</v>
+      </c>
       <c r="K809" t="s">
         <v>71</v>
       </c>
@@ -43956,6 +44158,9 @@
       <c r="I810" t="s">
         <v>48</v>
       </c>
+      <c r="J810">
+        <v>0</v>
+      </c>
       <c r="K810" t="s">
         <v>71</v>
       </c>
@@ -44006,6 +44211,9 @@
       <c r="I811" t="s">
         <v>66</v>
       </c>
+      <c r="J811">
+        <v>0</v>
+      </c>
       <c r="K811" t="s">
         <v>71</v>
       </c>
@@ -44056,6 +44264,9 @@
       <c r="I812" t="s">
         <v>17</v>
       </c>
+      <c r="J812">
+        <v>0</v>
+      </c>
       <c r="K812" t="s">
         <v>71</v>
       </c>
@@ -44106,6 +44317,9 @@
       <c r="I813" t="s">
         <v>24</v>
       </c>
+      <c r="J813">
+        <v>0</v>
+      </c>
       <c r="K813" t="s">
         <v>71</v>
       </c>
@@ -44156,6 +44370,9 @@
       <c r="I814" t="s">
         <v>24</v>
       </c>
+      <c r="J814">
+        <v>0</v>
+      </c>
       <c r="K814" t="s">
         <v>71</v>
       </c>
@@ -44206,6 +44423,9 @@
       <c r="I815" t="s">
         <v>16</v>
       </c>
+      <c r="J815">
+        <v>0</v>
+      </c>
       <c r="K815" t="s">
         <v>71</v>
       </c>
@@ -44255,6 +44475,9 @@
       </c>
       <c r="I816" t="s">
         <v>18</v>
+      </c>
+      <c r="J816">
+        <v>0</v>
       </c>
       <c r="K816" t="s">
         <v>71</v>
@@ -44306,6 +44529,9 @@
       <c r="I817" t="s">
         <v>17</v>
       </c>
+      <c r="J817">
+        <v>0</v>
+      </c>
       <c r="K817" t="s">
         <v>71</v>
       </c>
@@ -44356,6 +44582,9 @@
       <c r="I818" t="s">
         <v>35</v>
       </c>
+      <c r="J818">
+        <v>0</v>
+      </c>
       <c r="K818" t="s">
         <v>71</v>
       </c>
@@ -44406,6 +44635,9 @@
       <c r="I819" t="s">
         <v>4</v>
       </c>
+      <c r="J819">
+        <v>0</v>
+      </c>
       <c r="K819" t="s">
         <v>71</v>
       </c>
@@ -44456,6 +44688,9 @@
       <c r="I820" t="s">
         <v>32</v>
       </c>
+      <c r="J820">
+        <v>0</v>
+      </c>
       <c r="K820" t="s">
         <v>71</v>
       </c>
@@ -44506,6 +44741,9 @@
       <c r="I821" t="s">
         <v>38</v>
       </c>
+      <c r="J821">
+        <v>0</v>
+      </c>
       <c r="K821" t="s">
         <v>71</v>
       </c>
@@ -44556,6 +44794,9 @@
       <c r="I822" t="s">
         <v>39</v>
       </c>
+      <c r="J822">
+        <v>0</v>
+      </c>
       <c r="K822" t="s">
         <v>71</v>
       </c>
@@ -44606,6 +44847,9 @@
       <c r="I823" t="s">
         <v>1</v>
       </c>
+      <c r="J823">
+        <v>0</v>
+      </c>
       <c r="K823" t="s">
         <v>71</v>
       </c>
@@ -44656,6 +44900,9 @@
       <c r="I824" t="s">
         <v>24</v>
       </c>
+      <c r="J824">
+        <v>0</v>
+      </c>
       <c r="K824" t="s">
         <v>71</v>
       </c>
@@ -44706,6 +44953,9 @@
       <c r="I825" t="s">
         <v>11</v>
       </c>
+      <c r="J825">
+        <v>0</v>
+      </c>
       <c r="K825" t="s">
         <v>71</v>
       </c>
@@ -44756,6 +45006,9 @@
       <c r="I826" t="s">
         <v>29</v>
       </c>
+      <c r="J826">
+        <v>0</v>
+      </c>
       <c r="K826" t="s">
         <v>71</v>
       </c>
@@ -44806,6 +45059,9 @@
       <c r="I827" t="s">
         <v>6</v>
       </c>
+      <c r="J827">
+        <v>0</v>
+      </c>
       <c r="K827" t="s">
         <v>71</v>
       </c>
@@ -44856,6 +45112,9 @@
       <c r="I828" t="s">
         <v>10</v>
       </c>
+      <c r="J828">
+        <v>0</v>
+      </c>
       <c r="K828" t="s">
         <v>71</v>
       </c>
@@ -44906,6 +45165,9 @@
       <c r="I829" t="s">
         <v>0</v>
       </c>
+      <c r="J829">
+        <v>0</v>
+      </c>
       <c r="K829" t="s">
         <v>71</v>
       </c>
@@ -44956,6 +45218,9 @@
       <c r="I830" t="s">
         <v>11</v>
       </c>
+      <c r="J830">
+        <v>0</v>
+      </c>
       <c r="K830" t="s">
         <v>71</v>
       </c>
@@ -45006,6 +45271,9 @@
       <c r="I831" t="s">
         <v>6</v>
       </c>
+      <c r="J831">
+        <v>0</v>
+      </c>
       <c r="K831" t="s">
         <v>71</v>
       </c>
@@ -45056,6 +45324,9 @@
       <c r="I832" t="s">
         <v>12</v>
       </c>
+      <c r="J832">
+        <v>0</v>
+      </c>
       <c r="K832" t="s">
         <v>71</v>
       </c>
@@ -45106,6 +45377,9 @@
       <c r="I833" t="s">
         <v>29</v>
       </c>
+      <c r="J833">
+        <v>0</v>
+      </c>
       <c r="K833" t="s">
         <v>71</v>
       </c>
@@ -45155,6 +45429,9 @@
       </c>
       <c r="I834" t="s">
         <v>17</v>
+      </c>
+      <c r="J834">
+        <v>0</v>
       </c>
       <c r="K834" t="s">
         <v>71</v>
@@ -45206,6 +45483,9 @@
       <c r="I835" t="s">
         <v>1</v>
       </c>
+      <c r="J835">
+        <v>0</v>
+      </c>
       <c r="K835" t="s">
         <v>71</v>
       </c>
@@ -45256,6 +45536,9 @@
       <c r="I836" t="s">
         <v>11</v>
       </c>
+      <c r="J836">
+        <v>0</v>
+      </c>
       <c r="K836" t="s">
         <v>71</v>
       </c>
@@ -45306,6 +45589,9 @@
       <c r="I837" t="s">
         <v>12</v>
       </c>
+      <c r="J837">
+        <v>0</v>
+      </c>
       <c r="K837" t="s">
         <v>71</v>
       </c>
@@ -45356,6 +45642,9 @@
       <c r="I838" t="s">
         <v>52</v>
       </c>
+      <c r="J838">
+        <v>0</v>
+      </c>
       <c r="K838" t="s">
         <v>71</v>
       </c>
@@ -45406,6 +45695,9 @@
       <c r="I839" t="s">
         <v>23</v>
       </c>
+      <c r="J839">
+        <v>0</v>
+      </c>
       <c r="K839" t="s">
         <v>71</v>
       </c>
@@ -45456,6 +45748,9 @@
       <c r="I840" t="s">
         <v>1</v>
       </c>
+      <c r="J840">
+        <v>0</v>
+      </c>
       <c r="K840" t="s">
         <v>71</v>
       </c>
@@ -45506,6 +45801,9 @@
       <c r="I841" t="s">
         <v>23</v>
       </c>
+      <c r="J841">
+        <v>0</v>
+      </c>
       <c r="K841" t="s">
         <v>71</v>
       </c>
@@ -45556,6 +45854,9 @@
       <c r="I842" t="s">
         <v>10</v>
       </c>
+      <c r="J842">
+        <v>0</v>
+      </c>
       <c r="K842" t="s">
         <v>71</v>
       </c>
@@ -45606,6 +45907,9 @@
       <c r="I843" t="s">
         <v>18</v>
       </c>
+      <c r="J843">
+        <v>0</v>
+      </c>
       <c r="K843" t="s">
         <v>71</v>
       </c>
@@ -45656,6 +45960,9 @@
       <c r="I844" t="s">
         <v>18</v>
       </c>
+      <c r="J844">
+        <v>0</v>
+      </c>
       <c r="K844" t="s">
         <v>71</v>
       </c>
@@ -45706,6 +46013,9 @@
       <c r="I845" t="s">
         <v>11</v>
       </c>
+      <c r="J845">
+        <v>0</v>
+      </c>
       <c r="K845" t="s">
         <v>71</v>
       </c>
@@ -45756,6 +46066,9 @@
       <c r="I846" t="s">
         <v>17</v>
       </c>
+      <c r="J846">
+        <v>0</v>
+      </c>
       <c r="K846" t="s">
         <v>71</v>
       </c>
@@ -45806,6 +46119,9 @@
       <c r="I847" t="s">
         <v>21</v>
       </c>
+      <c r="J847">
+        <v>0</v>
+      </c>
       <c r="K847" t="s">
         <v>71</v>
       </c>
@@ -45856,6 +46172,9 @@
       <c r="I848" t="s">
         <v>50</v>
       </c>
+      <c r="J848">
+        <v>0</v>
+      </c>
       <c r="K848" t="s">
         <v>71</v>
       </c>
@@ -45906,6 +46225,9 @@
       <c r="I849" t="s">
         <v>23</v>
       </c>
+      <c r="J849">
+        <v>0</v>
+      </c>
       <c r="K849" t="s">
         <v>71</v>
       </c>
@@ -45956,6 +46278,9 @@
       <c r="I850" t="s">
         <v>8</v>
       </c>
+      <c r="J850">
+        <v>0</v>
+      </c>
       <c r="K850" t="s">
         <v>71</v>
       </c>
@@ -46005,6 +46330,9 @@
       </c>
       <c r="I851" t="s">
         <v>9</v>
+      </c>
+      <c r="J851">
+        <v>0</v>
       </c>
       <c r="K851" t="s">
         <v>71</v>
@@ -46056,6 +46384,9 @@
       <c r="I852" t="s">
         <v>7</v>
       </c>
+      <c r="J852">
+        <v>0</v>
+      </c>
       <c r="K852" t="s">
         <v>71</v>
       </c>
@@ -46106,6 +46437,9 @@
       <c r="I853" t="s">
         <v>22</v>
       </c>
+      <c r="J853">
+        <v>0</v>
+      </c>
       <c r="K853" t="s">
         <v>71</v>
       </c>
@@ -46156,6 +46490,9 @@
       <c r="I854" t="s">
         <v>18</v>
       </c>
+      <c r="J854">
+        <v>0</v>
+      </c>
       <c r="K854" t="s">
         <v>71</v>
       </c>
@@ -46206,6 +46543,9 @@
       <c r="I855" t="s">
         <v>0</v>
       </c>
+      <c r="J855">
+        <v>0</v>
+      </c>
       <c r="K855" t="s">
         <v>71</v>
       </c>
@@ -46256,6 +46596,9 @@
       <c r="I856" t="s">
         <v>42</v>
       </c>
+      <c r="J856">
+        <v>0</v>
+      </c>
       <c r="K856" t="s">
         <v>71</v>
       </c>
@@ -46306,6 +46649,9 @@
       <c r="I857" t="s">
         <v>0</v>
       </c>
+      <c r="J857">
+        <v>0</v>
+      </c>
       <c r="K857" t="s">
         <v>71</v>
       </c>
@@ -46356,6 +46702,9 @@
       <c r="I858" t="s">
         <v>15</v>
       </c>
+      <c r="J858">
+        <v>0</v>
+      </c>
       <c r="K858" t="s">
         <v>71</v>
       </c>
@@ -46406,6 +46755,9 @@
       <c r="I859" t="s">
         <v>11</v>
       </c>
+      <c r="J859">
+        <v>0</v>
+      </c>
       <c r="K859" t="s">
         <v>71</v>
       </c>
@@ -46456,6 +46808,9 @@
       <c r="I860" t="s">
         <v>65</v>
       </c>
+      <c r="J860">
+        <v>0</v>
+      </c>
       <c r="K860" t="s">
         <v>71</v>
       </c>
@@ -46506,6 +46861,9 @@
       <c r="I861" t="s">
         <v>59</v>
       </c>
+      <c r="J861">
+        <v>0</v>
+      </c>
       <c r="K861" t="s">
         <v>71</v>
       </c>
@@ -46556,6 +46914,9 @@
       <c r="I862" t="s">
         <v>19</v>
       </c>
+      <c r="J862">
+        <v>0</v>
+      </c>
       <c r="K862" t="s">
         <v>71</v>
       </c>
@@ -46606,6 +46967,9 @@
       <c r="I863" t="s">
         <v>23</v>
       </c>
+      <c r="J863">
+        <v>0</v>
+      </c>
       <c r="K863" t="s">
         <v>71</v>
       </c>
@@ -46656,6 +47020,9 @@
       <c r="I864" t="s">
         <v>20</v>
       </c>
+      <c r="J864">
+        <v>0</v>
+      </c>
       <c r="K864" t="s">
         <v>71</v>
       </c>
@@ -46706,6 +47073,9 @@
       <c r="I865" t="s">
         <v>18</v>
       </c>
+      <c r="J865">
+        <v>0</v>
+      </c>
       <c r="K865" t="s">
         <v>71</v>
       </c>
@@ -46756,6 +47126,9 @@
       <c r="I866" t="s">
         <v>18</v>
       </c>
+      <c r="J866">
+        <v>0</v>
+      </c>
       <c r="K866" t="s">
         <v>71</v>
       </c>
@@ -46806,6 +47179,9 @@
       <c r="I867" t="s">
         <v>27</v>
       </c>
+      <c r="J867">
+        <v>0</v>
+      </c>
       <c r="K867" t="s">
         <v>71</v>
       </c>
@@ -46856,6 +47232,9 @@
       <c r="I868" t="s">
         <v>28</v>
       </c>
+      <c r="J868">
+        <v>0</v>
+      </c>
       <c r="K868" t="s">
         <v>71</v>
       </c>
@@ -46906,6 +47285,9 @@
       <c r="I869" t="s">
         <v>1</v>
       </c>
+      <c r="J869">
+        <v>0</v>
+      </c>
       <c r="K869" t="s">
         <v>71</v>
       </c>
@@ -46955,6 +47337,9 @@
       </c>
       <c r="I870" t="s">
         <v>14</v>
+      </c>
+      <c r="J870">
+        <v>0</v>
       </c>
       <c r="K870" t="s">
         <v>71</v>
@@ -47006,6 +47391,9 @@
       <c r="I871" t="s">
         <v>16</v>
       </c>
+      <c r="J871">
+        <v>0</v>
+      </c>
       <c r="K871" t="s">
         <v>71</v>
       </c>
@@ -47056,6 +47444,9 @@
       <c r="I872" t="s">
         <v>17</v>
       </c>
+      <c r="J872">
+        <v>0</v>
+      </c>
       <c r="K872" t="s">
         <v>71</v>
       </c>
@@ -47106,6 +47497,9 @@
       <c r="I873" t="s">
         <v>12</v>
       </c>
+      <c r="J873">
+        <v>0</v>
+      </c>
       <c r="K873" t="s">
         <v>71</v>
       </c>
@@ -47156,6 +47550,9 @@
       <c r="I874" t="s">
         <v>3</v>
       </c>
+      <c r="J874">
+        <v>0</v>
+      </c>
       <c r="K874" t="s">
         <v>71</v>
       </c>
@@ -47206,6 +47603,9 @@
       <c r="I875" t="s">
         <v>16</v>
       </c>
+      <c r="J875">
+        <v>0</v>
+      </c>
       <c r="K875" t="s">
         <v>71</v>
       </c>
@@ -47256,6 +47656,9 @@
       <c r="I876" t="s">
         <v>17</v>
       </c>
+      <c r="J876">
+        <v>0</v>
+      </c>
       <c r="K876" t="s">
         <v>71</v>
       </c>
@@ -47306,6 +47709,9 @@
       <c r="I877" t="s">
         <v>6</v>
       </c>
+      <c r="J877">
+        <v>0</v>
+      </c>
       <c r="K877" t="s">
         <v>71</v>
       </c>
@@ -47356,6 +47762,9 @@
       <c r="I878" t="s">
         <v>16</v>
       </c>
+      <c r="J878">
+        <v>0</v>
+      </c>
       <c r="K878" t="s">
         <v>71</v>
       </c>
@@ -47406,6 +47815,9 @@
       <c r="I879" t="s">
         <v>14</v>
       </c>
+      <c r="J879">
+        <v>0</v>
+      </c>
       <c r="K879" t="s">
         <v>71</v>
       </c>
@@ -47456,6 +47868,9 @@
       <c r="I880" t="s">
         <v>6</v>
       </c>
+      <c r="J880">
+        <v>0</v>
+      </c>
       <c r="K880" t="s">
         <v>71</v>
       </c>
@@ -47506,6 +47921,9 @@
       <c r="I881" t="s">
         <v>29</v>
       </c>
+      <c r="J881">
+        <v>0</v>
+      </c>
       <c r="K881" t="s">
         <v>71</v>
       </c>
@@ -47556,6 +47974,9 @@
       <c r="I882" t="s">
         <v>4</v>
       </c>
+      <c r="J882">
+        <v>0</v>
+      </c>
       <c r="K882" t="s">
         <v>71</v>
       </c>
@@ -47606,6 +48027,9 @@
       <c r="I883" t="s">
         <v>0</v>
       </c>
+      <c r="J883">
+        <v>0</v>
+      </c>
       <c r="K883" t="s">
         <v>71</v>
       </c>
@@ -47656,6 +48080,9 @@
       <c r="I884" t="s">
         <v>54</v>
       </c>
+      <c r="J884">
+        <v>0</v>
+      </c>
       <c r="K884" t="s">
         <v>71</v>
       </c>
@@ -47706,6 +48133,9 @@
       <c r="I885" t="s">
         <v>17</v>
       </c>
+      <c r="J885">
+        <v>0</v>
+      </c>
       <c r="K885" t="s">
         <v>71</v>
       </c>
@@ -47756,6 +48186,9 @@
       <c r="I886" t="s">
         <v>4</v>
       </c>
+      <c r="J886">
+        <v>0</v>
+      </c>
       <c r="K886" t="s">
         <v>71</v>
       </c>
@@ -47805,6 +48238,9 @@
       </c>
       <c r="I887" t="s">
         <v>27</v>
+      </c>
+      <c r="J887">
+        <v>0</v>
       </c>
       <c r="K887" t="s">
         <v>71</v>
@@ -47856,6 +48292,9 @@
       <c r="I888" t="s">
         <v>69</v>
       </c>
+      <c r="J888">
+        <v>0</v>
+      </c>
       <c r="K888" t="s">
         <v>71</v>
       </c>
@@ -47906,6 +48345,9 @@
       <c r="I889" t="s">
         <v>9</v>
       </c>
+      <c r="J889">
+        <v>0</v>
+      </c>
       <c r="K889" t="s">
         <v>71</v>
       </c>
@@ -47956,6 +48398,9 @@
       <c r="I890" t="s">
         <v>29</v>
       </c>
+      <c r="J890">
+        <v>0</v>
+      </c>
       <c r="K890" t="s">
         <v>71</v>
       </c>
@@ -48006,6 +48451,9 @@
       <c r="I891" t="s">
         <v>53</v>
       </c>
+      <c r="J891">
+        <v>0</v>
+      </c>
       <c r="K891" t="s">
         <v>71</v>
       </c>
@@ -48056,6 +48504,9 @@
       <c r="I892" t="s">
         <v>27</v>
       </c>
+      <c r="J892">
+        <v>0</v>
+      </c>
       <c r="K892" t="s">
         <v>71</v>
       </c>
@@ -48106,6 +48557,9 @@
       <c r="I893" t="s">
         <v>21</v>
       </c>
+      <c r="J893">
+        <v>0</v>
+      </c>
       <c r="K893" t="s">
         <v>71</v>
       </c>
@@ -48156,6 +48610,9 @@
       <c r="I894" t="s">
         <v>34</v>
       </c>
+      <c r="J894">
+        <v>0</v>
+      </c>
       <c r="K894" t="s">
         <v>71</v>
       </c>
@@ -48206,6 +48663,9 @@
       <c r="I895" t="s">
         <v>24</v>
       </c>
+      <c r="J895">
+        <v>0</v>
+      </c>
       <c r="K895" t="s">
         <v>71</v>
       </c>
@@ -48256,6 +48716,9 @@
       <c r="I896" t="s">
         <v>55</v>
       </c>
+      <c r="J896">
+        <v>0</v>
+      </c>
       <c r="K896" t="s">
         <v>71</v>
       </c>
@@ -48306,6 +48769,9 @@
       <c r="I897" t="s">
         <v>28</v>
       </c>
+      <c r="J897">
+        <v>0</v>
+      </c>
       <c r="K897" t="s">
         <v>71</v>
       </c>
@@ -48356,6 +48822,9 @@
       <c r="I898" t="s">
         <v>48</v>
       </c>
+      <c r="J898">
+        <v>0</v>
+      </c>
       <c r="K898" t="s">
         <v>71</v>
       </c>
@@ -48406,6 +48875,9 @@
       <c r="I899" t="s">
         <v>14</v>
       </c>
+      <c r="J899">
+        <v>0</v>
+      </c>
       <c r="K899" t="s">
         <v>71</v>
       </c>
@@ -48456,6 +48928,9 @@
       <c r="I900" t="s">
         <v>3</v>
       </c>
+      <c r="J900">
+        <v>0</v>
+      </c>
       <c r="K900" t="s">
         <v>71</v>
       </c>
@@ -48506,6 +48981,9 @@
       <c r="I901" t="s">
         <v>22</v>
       </c>
+      <c r="J901">
+        <v>0</v>
+      </c>
       <c r="K901" t="s">
         <v>71</v>
       </c>
@@ -48556,6 +49034,9 @@
       <c r="I902" t="s">
         <v>6</v>
       </c>
+      <c r="J902">
+        <v>0</v>
+      </c>
       <c r="K902" t="s">
         <v>71</v>
       </c>
@@ -48606,6 +49087,9 @@
       <c r="I903" t="s">
         <v>24</v>
       </c>
+      <c r="J903">
+        <v>0</v>
+      </c>
       <c r="K903" t="s">
         <v>71</v>
       </c>
@@ -48656,6 +49140,9 @@
       <c r="I904" t="s">
         <v>52</v>
       </c>
+      <c r="J904">
+        <v>0</v>
+      </c>
       <c r="K904" t="s">
         <v>71</v>
       </c>
@@ -48706,6 +49193,9 @@
       <c r="I905" t="s">
         <v>18</v>
       </c>
+      <c r="J905">
+        <v>0</v>
+      </c>
       <c r="K905" t="s">
         <v>71</v>
       </c>
@@ -48755,6 +49245,9 @@
       </c>
       <c r="I906" t="s">
         <v>12</v>
+      </c>
+      <c r="J906">
+        <v>0</v>
       </c>
       <c r="K906" t="s">
         <v>71</v>
@@ -48806,6 +49299,9 @@
       <c r="I907" t="s">
         <v>14</v>
       </c>
+      <c r="J907">
+        <v>0</v>
+      </c>
       <c r="K907" t="s">
         <v>71</v>
       </c>
@@ -48856,6 +49352,9 @@
       <c r="I908" t="s">
         <v>11</v>
       </c>
+      <c r="J908">
+        <v>0</v>
+      </c>
       <c r="K908" t="s">
         <v>71</v>
       </c>
@@ -48906,6 +49405,9 @@
       <c r="I909" t="s">
         <v>18</v>
       </c>
+      <c r="J909">
+        <v>0</v>
+      </c>
       <c r="K909" t="s">
         <v>71</v>
       </c>
@@ -48956,6 +49458,9 @@
       <c r="I910" t="s">
         <v>3</v>
       </c>
+      <c r="J910">
+        <v>0</v>
+      </c>
       <c r="K910" t="s">
         <v>71</v>
       </c>
@@ -49006,6 +49511,9 @@
       <c r="I911" t="s">
         <v>18</v>
       </c>
+      <c r="J911">
+        <v>0</v>
+      </c>
       <c r="K911" t="s">
         <v>71</v>
       </c>
@@ -49056,6 +49564,9 @@
       <c r="I912" t="s">
         <v>16</v>
       </c>
+      <c r="J912">
+        <v>0</v>
+      </c>
       <c r="K912" t="s">
         <v>71</v>
       </c>
@@ -49106,6 +49617,9 @@
       <c r="I913" t="s">
         <v>17</v>
       </c>
+      <c r="J913">
+        <v>0</v>
+      </c>
       <c r="K913" t="s">
         <v>71</v>
       </c>
@@ -49156,6 +49670,9 @@
       <c r="I914" t="s">
         <v>29</v>
       </c>
+      <c r="J914">
+        <v>0</v>
+      </c>
       <c r="K914" t="s">
         <v>71</v>
       </c>
@@ -49206,6 +49723,9 @@
       <c r="I915" t="s">
         <v>4</v>
       </c>
+      <c r="J915">
+        <v>0</v>
+      </c>
       <c r="K915" t="s">
         <v>71</v>
       </c>
@@ -49256,6 +49776,9 @@
       <c r="I916" t="s">
         <v>23</v>
       </c>
+      <c r="J916">
+        <v>0</v>
+      </c>
       <c r="K916" t="s">
         <v>71</v>
       </c>
@@ -49306,6 +49829,9 @@
       <c r="I917" t="s">
         <v>29</v>
       </c>
+      <c r="J917">
+        <v>0</v>
+      </c>
       <c r="K917" t="s">
         <v>71</v>
       </c>
@@ -49356,6 +49882,9 @@
       <c r="I918" t="s">
         <v>38</v>
       </c>
+      <c r="J918">
+        <v>0</v>
+      </c>
       <c r="K918" t="s">
         <v>71</v>
       </c>
@@ -49406,6 +49935,9 @@
       <c r="I919" t="s">
         <v>19</v>
       </c>
+      <c r="J919">
+        <v>0</v>
+      </c>
       <c r="K919" t="s">
         <v>71</v>
       </c>
@@ -49456,6 +49988,9 @@
       <c r="I920" t="s">
         <v>23</v>
       </c>
+      <c r="J920">
+        <v>0</v>
+      </c>
       <c r="K920" t="s">
         <v>71</v>
       </c>
@@ -49506,6 +50041,9 @@
       <c r="I921" t="s">
         <v>1</v>
       </c>
+      <c r="J921">
+        <v>0</v>
+      </c>
       <c r="K921" t="s">
         <v>71</v>
       </c>
@@ -49556,6 +50094,9 @@
       <c r="I922" t="s">
         <v>11</v>
       </c>
+      <c r="J922">
+        <v>0</v>
+      </c>
       <c r="K922" t="s">
         <v>71</v>
       </c>
@@ -49606,6 +50147,9 @@
       <c r="I923" t="s">
         <v>29</v>
       </c>
+      <c r="J923">
+        <v>0</v>
+      </c>
       <c r="K923" t="s">
         <v>71</v>
       </c>
@@ -49655,6 +50199,9 @@
       </c>
       <c r="I924" t="s">
         <v>16</v>
+      </c>
+      <c r="J924">
+        <v>0</v>
       </c>
       <c r="K924" t="s">
         <v>71</v>
@@ -49706,6 +50253,9 @@
       <c r="I925" t="s">
         <v>9</v>
       </c>
+      <c r="J925">
+        <v>0</v>
+      </c>
       <c r="K925" t="s">
         <v>71</v>
       </c>
@@ -49756,6 +50306,9 @@
       <c r="I926" t="s">
         <v>1</v>
       </c>
+      <c r="J926">
+        <v>0</v>
+      </c>
       <c r="K926" t="s">
         <v>71</v>
       </c>
@@ -49806,6 +50359,9 @@
       <c r="I927" t="s">
         <v>10</v>
       </c>
+      <c r="J927">
+        <v>0</v>
+      </c>
       <c r="K927" t="s">
         <v>71</v>
       </c>
@@ -49856,6 +50412,9 @@
       <c r="I928" t="s">
         <v>28</v>
       </c>
+      <c r="J928">
+        <v>0</v>
+      </c>
       <c r="K928" t="s">
         <v>71</v>
       </c>
@@ -49906,6 +50465,9 @@
       <c r="I929" t="s">
         <v>11</v>
       </c>
+      <c r="J929">
+        <v>0</v>
+      </c>
       <c r="K929" t="s">
         <v>71</v>
       </c>
@@ -49956,6 +50518,9 @@
       <c r="I930" t="s">
         <v>45</v>
       </c>
+      <c r="J930">
+        <v>0</v>
+      </c>
       <c r="K930" t="s">
         <v>71</v>
       </c>
@@ -50006,6 +50571,9 @@
       <c r="I931" t="s">
         <v>21</v>
       </c>
+      <c r="J931">
+        <v>0</v>
+      </c>
       <c r="K931" t="s">
         <v>71</v>
       </c>
@@ -50056,6 +50624,9 @@
       <c r="I932" t="s">
         <v>36</v>
       </c>
+      <c r="J932">
+        <v>0</v>
+      </c>
       <c r="K932" t="s">
         <v>71</v>
       </c>
@@ -50106,6 +50677,9 @@
       <c r="I933" t="s">
         <v>12</v>
       </c>
+      <c r="J933">
+        <v>0</v>
+      </c>
       <c r="K933" t="s">
         <v>71</v>
       </c>
@@ -50156,6 +50730,9 @@
       <c r="I934" t="s">
         <v>10</v>
       </c>
+      <c r="J934">
+        <v>0</v>
+      </c>
       <c r="K934" t="s">
         <v>71</v>
       </c>
@@ -50206,6 +50783,9 @@
       <c r="I935" t="s">
         <v>34</v>
       </c>
+      <c r="J935">
+        <v>0</v>
+      </c>
       <c r="K935" t="s">
         <v>71</v>
       </c>
@@ -50256,6 +50836,9 @@
       <c r="I936" t="s">
         <v>22</v>
       </c>
+      <c r="J936">
+        <v>0</v>
+      </c>
       <c r="K936" t="s">
         <v>71</v>
       </c>
@@ -50306,6 +50889,9 @@
       <c r="I937" t="s">
         <v>10</v>
       </c>
+      <c r="J937">
+        <v>0</v>
+      </c>
       <c r="K937" t="s">
         <v>71</v>
       </c>
@@ -50356,6 +50942,9 @@
       <c r="I938" t="s">
         <v>45</v>
       </c>
+      <c r="J938">
+        <v>0</v>
+      </c>
       <c r="K938" t="s">
         <v>71</v>
       </c>
@@ -50406,6 +50995,9 @@
       <c r="I939" t="s">
         <v>4</v>
       </c>
+      <c r="J939">
+        <v>0</v>
+      </c>
       <c r="K939" t="s">
         <v>71</v>
       </c>
@@ -50456,6 +51048,9 @@
       <c r="I940" t="s">
         <v>41</v>
       </c>
+      <c r="J940">
+        <v>0</v>
+      </c>
       <c r="K940" t="s">
         <v>71</v>
       </c>
@@ -50506,6 +51101,9 @@
       <c r="I941" t="s">
         <v>15</v>
       </c>
+      <c r="J941">
+        <v>0</v>
+      </c>
       <c r="K941" t="s">
         <v>71</v>
       </c>
@@ -50555,6 +51153,9 @@
       </c>
       <c r="I942" t="s">
         <v>27</v>
+      </c>
+      <c r="J942">
+        <v>0</v>
       </c>
       <c r="K942" t="s">
         <v>71</v>
@@ -50606,6 +51207,9 @@
       <c r="I943" t="s">
         <v>4</v>
       </c>
+      <c r="J943">
+        <v>0</v>
+      </c>
       <c r="K943" t="s">
         <v>71</v>
       </c>
@@ -50656,6 +51260,9 @@
       <c r="I944" t="s">
         <v>22</v>
       </c>
+      <c r="J944">
+        <v>0</v>
+      </c>
       <c r="K944" t="s">
         <v>71</v>
       </c>
@@ -50706,6 +51313,9 @@
       <c r="I945" t="s">
         <v>47</v>
       </c>
+      <c r="J945">
+        <v>0</v>
+      </c>
       <c r="K945" t="s">
         <v>71</v>
       </c>
@@ -50756,6 +51366,9 @@
       <c r="I946" t="s">
         <v>28</v>
       </c>
+      <c r="J946">
+        <v>0</v>
+      </c>
       <c r="K946" t="s">
         <v>71</v>
       </c>
@@ -50806,6 +51419,9 @@
       <c r="I947" t="s">
         <v>12</v>
       </c>
+      <c r="J947">
+        <v>0</v>
+      </c>
       <c r="K947" t="s">
         <v>71</v>
       </c>
@@ -50856,6 +51472,9 @@
       <c r="I948" t="s">
         <v>12</v>
       </c>
+      <c r="J948">
+        <v>0</v>
+      </c>
       <c r="K948" t="s">
         <v>71</v>
       </c>
@@ -50906,6 +51525,9 @@
       <c r="I949" t="s">
         <v>22</v>
       </c>
+      <c r="J949">
+        <v>0</v>
+      </c>
       <c r="K949" t="s">
         <v>71</v>
       </c>
@@ -50956,6 +51578,9 @@
       <c r="I950" t="s">
         <v>9</v>
       </c>
+      <c r="J950">
+        <v>0</v>
+      </c>
       <c r="K950" t="s">
         <v>71</v>
       </c>
@@ -51006,6 +51631,9 @@
       <c r="I951" t="s">
         <v>44</v>
       </c>
+      <c r="J951">
+        <v>0</v>
+      </c>
       <c r="K951" t="s">
         <v>71</v>
       </c>
@@ -51056,6 +51684,9 @@
       <c r="I952" t="s">
         <v>19</v>
       </c>
+      <c r="J952">
+        <v>0</v>
+      </c>
       <c r="K952" t="s">
         <v>71</v>
       </c>
@@ -51106,6 +51737,9 @@
       <c r="I953" t="s">
         <v>27</v>
       </c>
+      <c r="J953">
+        <v>0</v>
+      </c>
       <c r="K953" t="s">
         <v>71</v>
       </c>
@@ -51156,6 +51790,9 @@
       <c r="I954" t="s">
         <v>44</v>
       </c>
+      <c r="J954">
+        <v>0</v>
+      </c>
       <c r="K954" t="s">
         <v>71</v>
       </c>
@@ -51206,6 +51843,9 @@
       <c r="I955" t="s">
         <v>22</v>
       </c>
+      <c r="J955">
+        <v>0</v>
+      </c>
       <c r="K955" t="s">
         <v>71</v>
       </c>
@@ -51256,6 +51896,9 @@
       <c r="I956" t="s">
         <v>14</v>
       </c>
+      <c r="J956">
+        <v>0</v>
+      </c>
       <c r="K956" t="s">
         <v>71</v>
       </c>
@@ -51306,6 +51949,9 @@
       <c r="I957" t="s">
         <v>9</v>
       </c>
+      <c r="J957">
+        <v>0</v>
+      </c>
       <c r="K957" t="s">
         <v>71</v>
       </c>
@@ -51356,6 +52002,9 @@
       <c r="I958" t="s">
         <v>40</v>
       </c>
+      <c r="J958">
+        <v>0</v>
+      </c>
       <c r="K958" t="s">
         <v>71</v>
       </c>
@@ -51406,6 +52055,9 @@
       <c r="I959" t="s">
         <v>17</v>
       </c>
+      <c r="J959">
+        <v>0</v>
+      </c>
       <c r="K959" t="s">
         <v>71</v>
       </c>
@@ -51456,6 +52108,9 @@
       <c r="I960" t="s">
         <v>4</v>
       </c>
+      <c r="J960">
+        <v>0</v>
+      </c>
       <c r="K960" t="s">
         <v>71</v>
       </c>
@@ -51506,6 +52161,9 @@
       <c r="I961" t="s">
         <v>24</v>
       </c>
+      <c r="J961">
+        <v>0</v>
+      </c>
       <c r="K961" t="s">
         <v>71</v>
       </c>
@@ -51556,6 +52214,9 @@
       <c r="I962" t="s">
         <v>12</v>
       </c>
+      <c r="J962">
+        <v>0</v>
+      </c>
       <c r="K962" t="s">
         <v>71</v>
       </c>
@@ -51606,6 +52267,9 @@
       <c r="I963" t="s">
         <v>9</v>
       </c>
+      <c r="J963">
+        <v>0</v>
+      </c>
       <c r="K963" t="s">
         <v>71</v>
       </c>
@@ -51656,6 +52320,9 @@
       <c r="I964" t="s">
         <v>19</v>
       </c>
+      <c r="J964">
+        <v>0</v>
+      </c>
       <c r="K964" t="s">
         <v>71</v>
       </c>
@@ -51706,6 +52373,9 @@
       <c r="I965" t="s">
         <v>9</v>
       </c>
+      <c r="J965">
+        <v>0</v>
+      </c>
       <c r="K965" t="s">
         <v>71</v>
       </c>
@@ -51755,6 +52425,9 @@
       </c>
       <c r="I966" t="s">
         <v>22</v>
+      </c>
+      <c r="J966">
+        <v>0</v>
       </c>
       <c r="K966" t="s">
         <v>71</v>
@@ -51806,6 +52479,9 @@
       <c r="I967" t="s">
         <v>1</v>
       </c>
+      <c r="J967">
+        <v>0</v>
+      </c>
       <c r="K967" t="s">
         <v>71</v>
       </c>
@@ -51856,6 +52532,9 @@
       <c r="I968" t="s">
         <v>17</v>
       </c>
+      <c r="J968">
+        <v>0</v>
+      </c>
       <c r="K968" t="s">
         <v>71</v>
       </c>
@@ -51906,6 +52585,9 @@
       <c r="I969" t="s">
         <v>42</v>
       </c>
+      <c r="J969">
+        <v>0</v>
+      </c>
       <c r="K969" t="s">
         <v>71</v>
       </c>
@@ -51956,6 +52638,9 @@
       <c r="I970" t="s">
         <v>2</v>
       </c>
+      <c r="J970">
+        <v>0</v>
+      </c>
       <c r="K970" t="s">
         <v>71</v>
       </c>
@@ -52006,6 +52691,9 @@
       <c r="I971" t="s">
         <v>12</v>
       </c>
+      <c r="J971">
+        <v>0</v>
+      </c>
       <c r="K971" t="s">
         <v>71</v>
       </c>
@@ -52056,6 +52744,9 @@
       <c r="I972" t="s">
         <v>17</v>
       </c>
+      <c r="J972">
+        <v>0</v>
+      </c>
       <c r="K972" t="s">
         <v>71</v>
       </c>
@@ -52106,6 +52797,9 @@
       <c r="I973" t="s">
         <v>3</v>
       </c>
+      <c r="J973">
+        <v>0</v>
+      </c>
       <c r="K973" t="s">
         <v>71</v>
       </c>
@@ -52156,6 +52850,9 @@
       <c r="I974" t="s">
         <v>4</v>
       </c>
+      <c r="J974">
+        <v>0</v>
+      </c>
       <c r="K974" t="s">
         <v>71</v>
       </c>
@@ -52206,6 +52903,9 @@
       <c r="I975" t="s">
         <v>24</v>
       </c>
+      <c r="J975">
+        <v>0</v>
+      </c>
       <c r="K975" t="s">
         <v>71</v>
       </c>
@@ -52256,6 +52956,9 @@
       <c r="I976" t="s">
         <v>27</v>
       </c>
+      <c r="J976">
+        <v>0</v>
+      </c>
       <c r="K976" t="s">
         <v>71</v>
       </c>
@@ -52306,6 +53009,9 @@
       <c r="I977" t="s">
         <v>44</v>
       </c>
+      <c r="J977">
+        <v>0</v>
+      </c>
       <c r="K977" t="s">
         <v>71</v>
       </c>
@@ -52356,6 +53062,9 @@
       <c r="I978" t="s">
         <v>32</v>
       </c>
+      <c r="J978">
+        <v>0</v>
+      </c>
       <c r="K978" t="s">
         <v>71</v>
       </c>
@@ -52406,6 +53115,9 @@
       <c r="I979" t="s">
         <v>51</v>
       </c>
+      <c r="J979">
+        <v>0</v>
+      </c>
       <c r="K979" t="s">
         <v>71</v>
       </c>
@@ -52456,6 +53168,9 @@
       <c r="I980" t="s">
         <v>17</v>
       </c>
+      <c r="J980">
+        <v>0</v>
+      </c>
       <c r="K980" t="s">
         <v>71</v>
       </c>
@@ -52506,6 +53221,9 @@
       <c r="I981" t="s">
         <v>12</v>
       </c>
+      <c r="J981">
+        <v>0</v>
+      </c>
       <c r="K981" t="s">
         <v>71</v>
       </c>
@@ -52556,6 +53274,9 @@
       <c r="I982" t="s">
         <v>21</v>
       </c>
+      <c r="J982">
+        <v>0</v>
+      </c>
       <c r="K982" t="s">
         <v>71</v>
       </c>
@@ -52606,6 +53327,9 @@
       <c r="I983" t="s">
         <v>27</v>
       </c>
+      <c r="J983">
+        <v>0</v>
+      </c>
       <c r="K983" t="s">
         <v>71</v>
       </c>
@@ -52656,6 +53380,9 @@
       <c r="I984" t="s">
         <v>2</v>
       </c>
+      <c r="J984">
+        <v>0</v>
+      </c>
       <c r="K984" t="s">
         <v>71</v>
       </c>
@@ -52706,6 +53433,9 @@
       <c r="I985" t="s">
         <v>59</v>
       </c>
+      <c r="J985">
+        <v>0</v>
+      </c>
       <c r="K985" t="s">
         <v>71</v>
       </c>
@@ -52756,6 +53486,9 @@
       <c r="I986" t="s">
         <v>14</v>
       </c>
+      <c r="J986">
+        <v>0</v>
+      </c>
       <c r="K986" t="s">
         <v>71</v>
       </c>
@@ -52805,6 +53538,9 @@
       </c>
       <c r="I987" t="s">
         <v>22</v>
+      </c>
+      <c r="J987">
+        <v>0</v>
       </c>
       <c r="K987" t="s">
         <v>71</v>
@@ -52856,6 +53592,9 @@
       <c r="I988" t="s">
         <v>8</v>
       </c>
+      <c r="J988">
+        <v>0</v>
+      </c>
       <c r="K988" t="s">
         <v>71</v>
       </c>
@@ -52906,6 +53645,9 @@
       <c r="I989" t="s">
         <v>18</v>
       </c>
+      <c r="J989">
+        <v>0</v>
+      </c>
       <c r="K989" t="s">
         <v>71</v>
       </c>
@@ -52956,6 +53698,9 @@
       <c r="I990" t="s">
         <v>21</v>
       </c>
+      <c r="J990">
+        <v>0</v>
+      </c>
       <c r="K990" t="s">
         <v>71</v>
       </c>
@@ -53006,6 +53751,9 @@
       <c r="I991" t="s">
         <v>5</v>
       </c>
+      <c r="J991">
+        <v>0</v>
+      </c>
       <c r="K991" t="s">
         <v>71</v>
       </c>
@@ -53056,6 +53804,9 @@
       <c r="I992" t="s">
         <v>18</v>
       </c>
+      <c r="J992">
+        <v>0</v>
+      </c>
       <c r="K992" t="s">
         <v>71</v>
       </c>
@@ -53106,6 +53857,9 @@
       <c r="I993" t="s">
         <v>18</v>
       </c>
+      <c r="J993">
+        <v>0</v>
+      </c>
       <c r="K993" t="s">
         <v>71</v>
       </c>
@@ -53156,6 +53910,9 @@
       <c r="I994" t="s">
         <v>10</v>
       </c>
+      <c r="J994">
+        <v>0</v>
+      </c>
       <c r="K994" t="s">
         <v>71</v>
       </c>
@@ -53206,6 +53963,9 @@
       <c r="I995" t="s">
         <v>29</v>
       </c>
+      <c r="J995">
+        <v>0</v>
+      </c>
       <c r="K995" t="s">
         <v>71</v>
       </c>
@@ -53256,6 +54016,9 @@
       <c r="I996" t="s">
         <v>24</v>
       </c>
+      <c r="J996">
+        <v>0</v>
+      </c>
       <c r="K996" t="s">
         <v>71</v>
       </c>
@@ -53306,6 +54069,9 @@
       <c r="I997" t="s">
         <v>14</v>
       </c>
+      <c r="J997">
+        <v>0</v>
+      </c>
       <c r="K997" t="s">
         <v>71</v>
       </c>
@@ -53356,6 +54122,9 @@
       <c r="I998" t="s">
         <v>6</v>
       </c>
+      <c r="J998">
+        <v>0</v>
+      </c>
       <c r="K998" t="s">
         <v>71</v>
       </c>
@@ -53406,6 +54175,9 @@
       <c r="I999" t="s">
         <v>30</v>
       </c>
+      <c r="J999">
+        <v>0</v>
+      </c>
       <c r="K999" t="s">
         <v>71</v>
       </c>
@@ -53456,6 +54228,9 @@
       <c r="I1000" t="s">
         <v>27</v>
       </c>
+      <c r="J1000">
+        <v>0</v>
+      </c>
       <c r="K1000" t="s">
         <v>71</v>
       </c>
@@ -53506,6 +54281,9 @@
       <c r="I1001" t="s">
         <v>36</v>
       </c>
+      <c r="J1001">
+        <v>0</v>
+      </c>
       <c r="K1001" t="s">
         <v>71</v>
       </c>
@@ -53556,6 +54334,9 @@
       <c r="I1002" t="s">
         <v>12</v>
       </c>
+      <c r="J1002">
+        <v>0</v>
+      </c>
       <c r="K1002" t="s">
         <v>71</v>
       </c>
@@ -53606,6 +54387,9 @@
       <c r="I1003" t="s">
         <v>15</v>
       </c>
+      <c r="J1003">
+        <v>0</v>
+      </c>
       <c r="K1003" t="s">
         <v>71</v>
       </c>
@@ -53656,6 +54440,9 @@
       <c r="I1004" t="s">
         <v>16</v>
       </c>
+      <c r="J1004">
+        <v>0</v>
+      </c>
       <c r="K1004" t="s">
         <v>71</v>
       </c>
@@ -53705,6 +54492,9 @@
       </c>
       <c r="I1005" t="s">
         <v>8</v>
+      </c>
+      <c r="J1005">
+        <v>0</v>
       </c>
       <c r="K1005" t="s">
         <v>71</v>
@@ -53756,6 +54546,9 @@
       <c r="I1006" t="s">
         <v>12</v>
       </c>
+      <c r="J1006">
+        <v>0</v>
+      </c>
       <c r="K1006" t="s">
         <v>71</v>
       </c>
@@ -53806,6 +54599,9 @@
       <c r="I1007" t="s">
         <v>16</v>
       </c>
+      <c r="J1007">
+        <v>0</v>
+      </c>
       <c r="K1007" t="s">
         <v>71</v>
       </c>
@@ -53856,6 +54652,9 @@
       <c r="I1008" t="s">
         <v>22</v>
       </c>
+      <c r="J1008">
+        <v>0</v>
+      </c>
       <c r="K1008" t="s">
         <v>71</v>
       </c>
@@ -53906,6 +54705,9 @@
       <c r="I1009" t="s">
         <v>17</v>
       </c>
+      <c r="J1009">
+        <v>0</v>
+      </c>
       <c r="K1009" t="s">
         <v>71</v>
       </c>
@@ -53956,6 +54758,9 @@
       <c r="I1010" t="s">
         <v>15</v>
       </c>
+      <c r="J1010">
+        <v>0</v>
+      </c>
       <c r="K1010" t="s">
         <v>71</v>
       </c>
@@ -54006,6 +54811,9 @@
       <c r="I1011" t="s">
         <v>15</v>
       </c>
+      <c r="J1011">
+        <v>0</v>
+      </c>
       <c r="K1011" t="s">
         <v>71</v>
       </c>
@@ -54056,6 +54864,9 @@
       <c r="I1012" t="s">
         <v>27</v>
       </c>
+      <c r="J1012">
+        <v>0</v>
+      </c>
       <c r="K1012" t="s">
         <v>71</v>
       </c>
@@ -54106,6 +54917,9 @@
       <c r="I1013" t="s">
         <v>23</v>
       </c>
+      <c r="J1013">
+        <v>0</v>
+      </c>
       <c r="K1013" t="s">
         <v>71</v>
       </c>
@@ -54156,6 +54970,9 @@
       <c r="I1014" t="s">
         <v>9</v>
       </c>
+      <c r="J1014">
+        <v>0</v>
+      </c>
       <c r="K1014" t="s">
         <v>71</v>
       </c>
@@ -54206,6 +55023,9 @@
       <c r="I1015" t="s">
         <v>24</v>
       </c>
+      <c r="J1015">
+        <v>0</v>
+      </c>
       <c r="K1015" t="s">
         <v>71</v>
       </c>
@@ -54256,6 +55076,9 @@
       <c r="I1016" t="s">
         <v>10</v>
       </c>
+      <c r="J1016">
+        <v>0</v>
+      </c>
       <c r="K1016" t="s">
         <v>71</v>
       </c>
@@ -54306,6 +55129,9 @@
       <c r="I1017" t="s">
         <v>9</v>
       </c>
+      <c r="J1017">
+        <v>0</v>
+      </c>
       <c r="K1017" t="s">
         <v>71</v>
       </c>
@@ -54356,6 +55182,9 @@
       <c r="I1018" t="s">
         <v>5</v>
       </c>
+      <c r="J1018">
+        <v>0</v>
+      </c>
       <c r="K1018" t="s">
         <v>71</v>
       </c>
@@ -54406,6 +55235,9 @@
       <c r="I1019" t="s">
         <v>8</v>
       </c>
+      <c r="J1019">
+        <v>0</v>
+      </c>
       <c r="K1019" t="s">
         <v>71</v>
       </c>
@@ -54456,6 +55288,9 @@
       <c r="I1020" t="s">
         <v>4</v>
       </c>
+      <c r="J1020">
+        <v>0</v>
+      </c>
       <c r="K1020" t="s">
         <v>71</v>
       </c>
@@ -54506,6 +55341,9 @@
       <c r="I1021" t="s">
         <v>24</v>
       </c>
+      <c r="J1021">
+        <v>0</v>
+      </c>
       <c r="K1021" t="s">
         <v>71</v>
       </c>
@@ -54555,6 +55393,9 @@
       </c>
       <c r="I1022" t="s">
         <v>5</v>
+      </c>
+      <c r="J1022">
+        <v>0</v>
       </c>
       <c r="K1022" t="s">
         <v>71</v>
@@ -54606,6 +55447,9 @@
       <c r="I1023" t="s">
         <v>33</v>
       </c>
+      <c r="J1023">
+        <v>0</v>
+      </c>
       <c r="K1023" t="s">
         <v>71</v>
       </c>
@@ -54656,6 +55500,9 @@
       <c r="I1024" t="s">
         <v>3</v>
       </c>
+      <c r="J1024">
+        <v>0</v>
+      </c>
       <c r="K1024" t="s">
         <v>71</v>
       </c>
@@ -54706,6 +55553,9 @@
       <c r="I1025" t="s">
         <v>47</v>
       </c>
+      <c r="J1025">
+        <v>0</v>
+      </c>
       <c r="K1025" t="s">
         <v>71</v>
       </c>
@@ -54756,6 +55606,9 @@
       <c r="I1026" t="s">
         <v>9</v>
       </c>
+      <c r="J1026">
+        <v>0</v>
+      </c>
       <c r="K1026" t="s">
         <v>71</v>
       </c>
@@ -54806,6 +55659,9 @@
       <c r="I1027" t="s">
         <v>24</v>
       </c>
+      <c r="J1027">
+        <v>0</v>
+      </c>
       <c r="K1027" t="s">
         <v>71</v>
       </c>
@@ -54856,6 +55712,9 @@
       <c r="I1028" t="s">
         <v>3</v>
       </c>
+      <c r="J1028">
+        <v>0</v>
+      </c>
       <c r="K1028" t="s">
         <v>71</v>
       </c>
@@ -54906,6 +55765,9 @@
       <c r="I1029" t="s">
         <v>23</v>
       </c>
+      <c r="J1029">
+        <v>0</v>
+      </c>
       <c r="K1029" t="s">
         <v>71</v>
       </c>
@@ -54956,6 +55818,9 @@
       <c r="I1030" t="s">
         <v>6</v>
       </c>
+      <c r="J1030">
+        <v>0</v>
+      </c>
       <c r="K1030" t="s">
         <v>71</v>
       </c>
@@ -55006,6 +55871,9 @@
       <c r="I1031" t="s">
         <v>27</v>
       </c>
+      <c r="J1031">
+        <v>0</v>
+      </c>
       <c r="K1031" t="s">
         <v>71</v>
       </c>
@@ -55056,6 +55924,9 @@
       <c r="I1032" t="s">
         <v>17</v>
       </c>
+      <c r="J1032">
+        <v>0</v>
+      </c>
       <c r="K1032" t="s">
         <v>71</v>
       </c>
@@ -55106,6 +55977,9 @@
       <c r="I1033" t="s">
         <v>6</v>
       </c>
+      <c r="J1033">
+        <v>0</v>
+      </c>
       <c r="K1033" t="s">
         <v>71</v>
       </c>
@@ -55156,6 +56030,9 @@
       <c r="I1034" t="s">
         <v>7</v>
       </c>
+      <c r="J1034">
+        <v>0</v>
+      </c>
       <c r="K1034" t="s">
         <v>71</v>
       </c>
@@ -55206,6 +56083,9 @@
       <c r="I1035" t="s">
         <v>2</v>
       </c>
+      <c r="J1035">
+        <v>0</v>
+      </c>
       <c r="K1035" t="s">
         <v>71</v>
       </c>
@@ -55256,6 +56136,9 @@
       <c r="I1036" t="s">
         <v>17</v>
       </c>
+      <c r="J1036">
+        <v>0</v>
+      </c>
       <c r="K1036" t="s">
         <v>71</v>
       </c>
@@ -55306,6 +56189,9 @@
       <c r="I1037" t="s">
         <v>22</v>
       </c>
+      <c r="J1037">
+        <v>0</v>
+      </c>
       <c r="K1037" t="s">
         <v>71</v>
       </c>
@@ -55355,6 +56241,9 @@
       </c>
       <c r="I1038" t="s">
         <v>42</v>
+      </c>
+      <c r="J1038">
+        <v>0</v>
       </c>
       <c r="K1038" t="s">
         <v>71</v>
@@ -55406,6 +56295,9 @@
       <c r="I1039" t="s">
         <v>8</v>
       </c>
+      <c r="J1039">
+        <v>0</v>
+      </c>
       <c r="K1039" t="s">
         <v>71</v>
       </c>
@@ -55456,6 +56348,9 @@
       <c r="I1040" t="s">
         <v>41</v>
       </c>
+      <c r="J1040">
+        <v>0</v>
+      </c>
       <c r="K1040" t="s">
         <v>71</v>
       </c>
@@ -55506,6 +56401,9 @@
       <c r="I1041" t="s">
         <v>21</v>
       </c>
+      <c r="J1041">
+        <v>0</v>
+      </c>
       <c r="K1041" t="s">
         <v>71</v>
       </c>
@@ -55556,6 +56454,9 @@
       <c r="I1042" t="s">
         <v>47</v>
       </c>
+      <c r="J1042">
+        <v>0</v>
+      </c>
       <c r="K1042" t="s">
         <v>71</v>
       </c>
@@ -55606,6 +56507,9 @@
       <c r="I1043" t="s">
         <v>12</v>
       </c>
+      <c r="J1043">
+        <v>0</v>
+      </c>
       <c r="K1043" t="s">
         <v>71</v>
       </c>
@@ -55656,6 +56560,9 @@
       <c r="I1044" t="s">
         <v>54</v>
       </c>
+      <c r="J1044">
+        <v>0</v>
+      </c>
       <c r="K1044" t="s">
         <v>71</v>
       </c>
@@ -55706,6 +56613,9 @@
       <c r="I1045" t="s">
         <v>15</v>
       </c>
+      <c r="J1045">
+        <v>0</v>
+      </c>
       <c r="K1045" t="s">
         <v>71</v>
       </c>
@@ -55756,6 +56666,9 @@
       <c r="I1046" t="s">
         <v>5</v>
       </c>
+      <c r="J1046">
+        <v>0</v>
+      </c>
       <c r="K1046" t="s">
         <v>71</v>
       </c>
@@ -55806,6 +56719,9 @@
       <c r="I1047" t="s">
         <v>49</v>
       </c>
+      <c r="J1047">
+        <v>0</v>
+      </c>
       <c r="K1047" t="s">
         <v>71</v>
       </c>
@@ -55856,6 +56772,9 @@
       <c r="I1048" t="s">
         <v>61</v>
       </c>
+      <c r="J1048">
+        <v>0</v>
+      </c>
       <c r="K1048" t="s">
         <v>71</v>
       </c>
@@ -55906,6 +56825,9 @@
       <c r="I1049" t="s">
         <v>41</v>
       </c>
+      <c r="J1049">
+        <v>0</v>
+      </c>
       <c r="K1049" t="s">
         <v>71</v>
       </c>
@@ -55956,6 +56878,9 @@
       <c r="I1050" t="s">
         <v>46</v>
       </c>
+      <c r="J1050">
+        <v>0</v>
+      </c>
       <c r="K1050" t="s">
         <v>71</v>
       </c>
@@ -56006,6 +56931,9 @@
       <c r="I1051" t="s">
         <v>62</v>
       </c>
+      <c r="J1051">
+        <v>0</v>
+      </c>
       <c r="K1051" t="s">
         <v>71</v>
       </c>
@@ -56056,6 +56984,9 @@
       <c r="I1052" t="s">
         <v>33</v>
       </c>
+      <c r="J1052">
+        <v>0</v>
+      </c>
       <c r="K1052" t="s">
         <v>71</v>
       </c>
@@ -56106,6 +57037,9 @@
       <c r="I1053" t="s">
         <v>2</v>
       </c>
+      <c r="J1053">
+        <v>0</v>
+      </c>
       <c r="K1053" t="s">
         <v>71</v>
       </c>
@@ -56155,6 +57089,9 @@
       </c>
       <c r="I1054" t="s">
         <v>25</v>
+      </c>
+      <c r="J1054">
+        <v>0</v>
       </c>
       <c r="K1054" t="s">
         <v>71</v>
@@ -56206,6 +57143,9 @@
       <c r="I1055" t="s">
         <v>28</v>
       </c>
+      <c r="J1055">
+        <v>0</v>
+      </c>
       <c r="K1055" t="s">
         <v>71</v>
       </c>
@@ -56256,6 +57196,9 @@
       <c r="I1056" t="s">
         <v>28</v>
       </c>
+      <c r="J1056">
+        <v>0</v>
+      </c>
       <c r="K1056" t="s">
         <v>71</v>
       </c>
@@ -56306,6 +57249,9 @@
       <c r="I1057" t="s">
         <v>26</v>
       </c>
+      <c r="J1057">
+        <v>0</v>
+      </c>
       <c r="K1057" t="s">
         <v>71</v>
       </c>
@@ -56356,6 +57302,9 @@
       <c r="I1058" t="s">
         <v>33</v>
       </c>
+      <c r="J1058">
+        <v>0</v>
+      </c>
       <c r="K1058" t="s">
         <v>71</v>
       </c>
@@ -56406,6 +57355,9 @@
       <c r="I1059" t="s">
         <v>3</v>
       </c>
+      <c r="J1059">
+        <v>0</v>
+      </c>
       <c r="K1059" t="s">
         <v>71</v>
       </c>
@@ -56456,6 +57408,9 @@
       <c r="I1060" t="s">
         <v>7</v>
       </c>
+      <c r="J1060">
+        <v>0</v>
+      </c>
       <c r="K1060" t="s">
         <v>71</v>
       </c>
@@ -56506,6 +57461,9 @@
       <c r="I1061" t="s">
         <v>44</v>
       </c>
+      <c r="J1061">
+        <v>0</v>
+      </c>
       <c r="K1061" t="s">
         <v>71</v>
       </c>
@@ -56556,6 +57514,9 @@
       <c r="I1062" t="s">
         <v>22</v>
       </c>
+      <c r="J1062">
+        <v>0</v>
+      </c>
       <c r="K1062" t="s">
         <v>71</v>
       </c>
@@ -56606,6 +57567,9 @@
       <c r="I1063" t="s">
         <v>19</v>
       </c>
+      <c r="J1063">
+        <v>0</v>
+      </c>
       <c r="K1063" t="s">
         <v>71</v>
       </c>
@@ -56656,6 +57620,9 @@
       <c r="I1064" t="s">
         <v>21</v>
       </c>
+      <c r="J1064">
+        <v>0</v>
+      </c>
       <c r="K1064" t="s">
         <v>71</v>
       </c>
@@ -56706,6 +57673,9 @@
       <c r="I1065" t="s">
         <v>33</v>
       </c>
+      <c r="J1065">
+        <v>0</v>
+      </c>
       <c r="K1065" t="s">
         <v>71</v>
       </c>
@@ -56756,6 +57726,9 @@
       <c r="I1066" t="s">
         <v>0</v>
       </c>
+      <c r="J1066">
+        <v>0</v>
+      </c>
       <c r="K1066" t="s">
         <v>71</v>
       </c>
@@ -56806,6 +57779,9 @@
       <c r="I1067" t="s">
         <v>51</v>
       </c>
+      <c r="J1067">
+        <v>0</v>
+      </c>
       <c r="K1067" t="s">
         <v>71</v>
       </c>
@@ -56856,6 +57832,9 @@
       <c r="I1068" t="s">
         <v>24</v>
       </c>
+      <c r="J1068">
+        <v>0</v>
+      </c>
       <c r="K1068" t="s">
         <v>71</v>
       </c>
@@ -56906,6 +57885,9 @@
       <c r="I1069" t="s">
         <v>2</v>
       </c>
+      <c r="J1069">
+        <v>0</v>
+      </c>
       <c r="K1069" t="s">
         <v>71</v>
       </c>
@@ -56955,6 +57937,9 @@
       </c>
       <c r="I1070" t="s">
         <v>47</v>
+      </c>
+      <c r="J1070">
+        <v>0</v>
       </c>
       <c r="K1070" t="s">
         <v>71</v>
@@ -57006,6 +57991,9 @@
       <c r="I1071" t="s">
         <v>27</v>
       </c>
+      <c r="J1071">
+        <v>0</v>
+      </c>
       <c r="K1071" t="s">
         <v>71</v>
       </c>
@@ -57056,6 +58044,9 @@
       <c r="I1072" t="s">
         <v>33</v>
       </c>
+      <c r="J1072">
+        <v>0</v>
+      </c>
       <c r="K1072" t="s">
         <v>71</v>
       </c>
@@ -57106,6 +58097,9 @@
       <c r="I1073" t="s">
         <v>47</v>
       </c>
+      <c r="J1073">
+        <v>0</v>
+      </c>
       <c r="K1073" t="s">
         <v>71</v>
       </c>
@@ -57156,6 +58150,9 @@
       <c r="I1074" t="s">
         <v>52</v>
       </c>
+      <c r="J1074">
+        <v>0</v>
+      </c>
       <c r="K1074" t="s">
         <v>71</v>
       </c>
@@ -57206,6 +58203,9 @@
       <c r="I1075" t="s">
         <v>5</v>
       </c>
+      <c r="J1075">
+        <v>0</v>
+      </c>
       <c r="K1075" t="s">
         <v>71</v>
       </c>
@@ -57256,6 +58256,9 @@
       <c r="I1076" t="s">
         <v>21</v>
       </c>
+      <c r="J1076">
+        <v>0</v>
+      </c>
       <c r="K1076" t="s">
         <v>71</v>
       </c>
@@ -57306,6 +58309,9 @@
       <c r="I1077" t="s">
         <v>25</v>
       </c>
+      <c r="J1077">
+        <v>0</v>
+      </c>
       <c r="K1077" t="s">
         <v>71</v>
       </c>
@@ -57356,6 +58362,9 @@
       <c r="I1078" t="s">
         <v>49</v>
       </c>
+      <c r="J1078">
+        <v>0</v>
+      </c>
       <c r="K1078" t="s">
         <v>71</v>
       </c>
@@ -57406,6 +58415,9 @@
       <c r="I1079" t="s">
         <v>51</v>
       </c>
+      <c r="J1079">
+        <v>0</v>
+      </c>
       <c r="K1079" t="s">
         <v>71</v>
       </c>
@@ -57456,6 +58468,9 @@
       <c r="I1080" t="s">
         <v>15</v>
       </c>
+      <c r="J1080">
+        <v>0</v>
+      </c>
       <c r="K1080" t="s">
         <v>71</v>
       </c>
@@ -57506,6 +58521,9 @@
       <c r="I1081" t="s">
         <v>61</v>
       </c>
+      <c r="J1081">
+        <v>0</v>
+      </c>
       <c r="K1081" t="s">
         <v>71</v>
       </c>
@@ -57556,6 +58574,9 @@
       <c r="I1082" t="s">
         <v>42</v>
       </c>
+      <c r="J1082">
+        <v>0</v>
+      </c>
       <c r="K1082" t="s">
         <v>71</v>
       </c>
@@ -57606,6 +58627,9 @@
       <c r="I1083" t="s">
         <v>5</v>
       </c>
+      <c r="J1083">
+        <v>0</v>
+      </c>
       <c r="K1083" t="s">
         <v>71</v>
       </c>
@@ -57656,6 +58680,9 @@
       <c r="I1084" t="s">
         <v>55</v>
       </c>
+      <c r="J1084">
+        <v>0</v>
+      </c>
       <c r="K1084" t="s">
         <v>71</v>
       </c>
@@ -57706,6 +58733,9 @@
       <c r="I1085" t="s">
         <v>25</v>
       </c>
+      <c r="J1085">
+        <v>0</v>
+      </c>
       <c r="K1085" t="s">
         <v>71</v>
       </c>
@@ -57756,6 +58786,9 @@
       <c r="I1086" t="s">
         <v>2</v>
       </c>
+      <c r="J1086">
+        <v>0</v>
+      </c>
       <c r="K1086" t="s">
         <v>71</v>
       </c>
@@ -57805,6 +58838,9 @@
       </c>
       <c r="I1087" t="s">
         <v>7</v>
+      </c>
+      <c r="J1087">
+        <v>0</v>
       </c>
       <c r="K1087" t="s">
         <v>71</v>
@@ -57856,6 +58892,9 @@
       <c r="I1088" t="s">
         <v>32</v>
       </c>
+      <c r="J1088">
+        <v>0</v>
+      </c>
       <c r="K1088" t="s">
         <v>71</v>
       </c>
@@ -57906,6 +58945,9 @@
       <c r="I1089" t="s">
         <v>5</v>
       </c>
+      <c r="J1089">
+        <v>0</v>
+      </c>
       <c r="K1089" t="s">
         <v>71</v>
       </c>
@@ -57956,6 +58998,9 @@
       <c r="I1090" t="s">
         <v>7</v>
       </c>
+      <c r="J1090">
+        <v>0</v>
+      </c>
       <c r="K1090" t="s">
         <v>71</v>
       </c>
@@ -58006,6 +59051,9 @@
       <c r="I1091" t="s">
         <v>3</v>
       </c>
+      <c r="J1091">
+        <v>0</v>
+      </c>
       <c r="K1091" t="s">
         <v>71</v>
       </c>
@@ -58056,6 +59104,9 @@
       <c r="I1092" t="s">
         <v>27</v>
       </c>
+      <c r="J1092">
+        <v>0</v>
+      </c>
       <c r="K1092" t="s">
         <v>71</v>
       </c>
@@ -58106,6 +59157,9 @@
       <c r="I1093" t="s">
         <v>41</v>
       </c>
+      <c r="J1093">
+        <v>0</v>
+      </c>
       <c r="K1093" t="s">
         <v>71</v>
       </c>
@@ -58156,6 +59210,9 @@
       <c r="I1094" t="s">
         <v>53</v>
       </c>
+      <c r="J1094">
+        <v>0</v>
+      </c>
       <c r="K1094" t="s">
         <v>71</v>
       </c>
@@ -58206,6 +59263,9 @@
       <c r="I1095" t="s">
         <v>0</v>
       </c>
+      <c r="J1095">
+        <v>0</v>
+      </c>
       <c r="K1095" t="s">
         <v>71</v>
       </c>
@@ -58256,6 +59316,9 @@
       <c r="I1096" t="s">
         <v>25</v>
       </c>
+      <c r="J1096">
+        <v>0</v>
+      </c>
       <c r="K1096" t="s">
         <v>71</v>
       </c>
@@ -58306,6 +59369,9 @@
       <c r="I1097" t="s">
         <v>0</v>
       </c>
+      <c r="J1097">
+        <v>0</v>
+      </c>
       <c r="K1097" t="s">
         <v>71</v>
       </c>
@@ -58356,6 +59422,9 @@
       <c r="I1098" t="s">
         <v>25</v>
       </c>
+      <c r="J1098">
+        <v>0</v>
+      </c>
       <c r="K1098" t="s">
         <v>71</v>
       </c>
@@ -58406,6 +59475,9 @@
       <c r="I1099" t="s">
         <v>2</v>
       </c>
+      <c r="J1099">
+        <v>0</v>
+      </c>
       <c r="K1099" t="s">
         <v>71</v>
       </c>
@@ -58456,6 +59528,9 @@
       <c r="I1100" t="s">
         <v>31</v>
       </c>
+      <c r="J1100">
+        <v>0</v>
+      </c>
       <c r="K1100" t="s">
         <v>71</v>
       </c>
@@ -58506,6 +59581,9 @@
       <c r="I1101" t="s">
         <v>33</v>
       </c>
+      <c r="J1101">
+        <v>0</v>
+      </c>
       <c r="K1101" t="s">
         <v>71</v>
       </c>
@@ -58556,6 +59634,9 @@
       <c r="I1102" t="s">
         <v>13</v>
       </c>
+      <c r="J1102">
+        <v>0</v>
+      </c>
       <c r="K1102" t="s">
         <v>71</v>
       </c>
@@ -58605,6 +59686,9 @@
       </c>
       <c r="I1103" t="s">
         <v>47</v>
+      </c>
+      <c r="J1103">
+        <v>0</v>
       </c>
       <c r="K1103" t="s">
         <v>71</v>
@@ -58656,6 +59740,9 @@
       <c r="I1104" t="s">
         <v>13</v>
       </c>
+      <c r="J1104">
+        <v>0</v>
+      </c>
       <c r="K1104" t="s">
         <v>71</v>
       </c>
@@ -58706,6 +59793,9 @@
       <c r="I1105" t="s">
         <v>3</v>
       </c>
+      <c r="J1105">
+        <v>0</v>
+      </c>
       <c r="K1105" t="s">
         <v>71</v>
       </c>
@@ -58756,6 +59846,9 @@
       <c r="I1106" t="s">
         <v>0</v>
       </c>
+      <c r="J1106">
+        <v>0</v>
+      </c>
       <c r="K1106" t="s">
         <v>71</v>
       </c>
@@ -58806,6 +59899,9 @@
       <c r="I1107" t="s">
         <v>21</v>
       </c>
+      <c r="J1107">
+        <v>0</v>
+      </c>
       <c r="K1107" t="s">
         <v>71</v>
       </c>
@@ -58856,6 +59952,9 @@
       <c r="I1108" t="s">
         <v>47</v>
       </c>
+      <c r="J1108">
+        <v>0</v>
+      </c>
       <c r="K1108" t="s">
         <v>71</v>
       </c>
@@ -58906,6 +60005,9 @@
       <c r="I1109" t="s">
         <v>47</v>
       </c>
+      <c r="J1109">
+        <v>0</v>
+      </c>
       <c r="K1109" t="s">
         <v>71</v>
       </c>
@@ -58956,6 +60058,9 @@
       <c r="I1110" t="s">
         <v>0</v>
       </c>
+      <c r="J1110">
+        <v>0</v>
+      </c>
       <c r="K1110" t="s">
         <v>71</v>
       </c>
@@ -59006,6 +60111,9 @@
       <c r="I1111" t="s">
         <v>4</v>
       </c>
+      <c r="J1111">
+        <v>0</v>
+      </c>
       <c r="K1111" t="s">
         <v>71</v>
       </c>
@@ -59056,6 +60164,9 @@
       <c r="I1112" t="s">
         <v>6</v>
       </c>
+      <c r="J1112">
+        <v>0</v>
+      </c>
       <c r="K1112" t="s">
         <v>71</v>
       </c>
@@ -59106,6 +60217,9 @@
       <c r="I1113" t="s">
         <v>32</v>
       </c>
+      <c r="J1113">
+        <v>0</v>
+      </c>
       <c r="K1113" t="s">
         <v>71</v>
       </c>
@@ -59156,6 +60270,9 @@
       <c r="I1114" t="s">
         <v>1</v>
       </c>
+      <c r="J1114">
+        <v>0</v>
+      </c>
       <c r="K1114" t="s">
         <v>71</v>
       </c>
@@ -59206,6 +60323,9 @@
       <c r="I1115" t="s">
         <v>12</v>
       </c>
+      <c r="J1115">
+        <v>0</v>
+      </c>
       <c r="K1115" t="s">
         <v>71</v>
       </c>
@@ -59256,6 +60376,9 @@
       <c r="I1116" t="s">
         <v>0</v>
       </c>
+      <c r="J1116">
+        <v>0</v>
+      </c>
       <c r="K1116" t="s">
         <v>71</v>
       </c>
@@ -59306,6 +60429,9 @@
       <c r="I1117" t="s">
         <v>44</v>
       </c>
+      <c r="J1117">
+        <v>0</v>
+      </c>
       <c r="K1117" t="s">
         <v>71</v>
       </c>
@@ -59355,6 +60481,9 @@
       </c>
       <c r="I1118" t="s">
         <v>17</v>
+      </c>
+      <c r="J1118">
+        <v>0</v>
       </c>
       <c r="K1118" t="s">
         <v>71</v>
@@ -59406,6 +60535,9 @@
       <c r="I1119" t="s">
         <v>9</v>
       </c>
+      <c r="J1119">
+        <v>0</v>
+      </c>
       <c r="K1119" t="s">
         <v>71</v>
       </c>
@@ -59456,6 +60588,9 @@
       <c r="I1120" t="s">
         <v>9</v>
       </c>
+      <c r="J1120">
+        <v>0</v>
+      </c>
       <c r="K1120" t="s">
         <v>71</v>
       </c>
@@ -59506,6 +60641,9 @@
       <c r="I1121" t="s">
         <v>14</v>
       </c>
+      <c r="J1121">
+        <v>0</v>
+      </c>
       <c r="K1121" t="s">
         <v>71</v>
       </c>
@@ -59556,6 +60694,9 @@
       <c r="I1122" t="s">
         <v>47</v>
       </c>
+      <c r="J1122">
+        <v>0</v>
+      </c>
       <c r="K1122" t="s">
         <v>71</v>
       </c>
@@ -59606,6 +60747,9 @@
       <c r="I1123" t="s">
         <v>4</v>
       </c>
+      <c r="J1123">
+        <v>0</v>
+      </c>
       <c r="K1123" t="s">
         <v>71</v>
       </c>
@@ -59656,6 +60800,9 @@
       <c r="I1124" t="s">
         <v>24</v>
       </c>
+      <c r="J1124">
+        <v>0</v>
+      </c>
       <c r="K1124" t="s">
         <v>71</v>
       </c>
@@ -59706,6 +60853,9 @@
       <c r="I1125" t="s">
         <v>12</v>
       </c>
+      <c r="J1125">
+        <v>0</v>
+      </c>
       <c r="K1125" t="s">
         <v>71</v>
       </c>
@@ -59756,6 +60906,9 @@
       <c r="I1126" t="s">
         <v>24</v>
       </c>
+      <c r="J1126">
+        <v>0</v>
+      </c>
       <c r="K1126" t="s">
         <v>71</v>
       </c>
@@ -59806,6 +60959,9 @@
       <c r="I1127" t="s">
         <v>44</v>
       </c>
+      <c r="J1127">
+        <v>0</v>
+      </c>
       <c r="K1127" t="s">
         <v>71</v>
       </c>
@@ -59856,6 +61012,9 @@
       <c r="I1128" t="s">
         <v>27</v>
       </c>
+      <c r="J1128">
+        <v>0</v>
+      </c>
       <c r="K1128" t="s">
         <v>71</v>
       </c>
@@ -59906,6 +61065,9 @@
       <c r="I1129" t="s">
         <v>22</v>
       </c>
+      <c r="J1129">
+        <v>0</v>
+      </c>
       <c r="K1129" t="s">
         <v>71</v>
       </c>
@@ -59955,6 +61117,9 @@
       </c>
       <c r="I1130" t="s">
         <v>20</v>
+      </c>
+      <c r="J1130">
+        <v>0</v>
       </c>
       <c r="K1130" t="s">
         <v>71</v>
@@ -60006,6 +61171,9 @@
       <c r="I1131" t="s">
         <v>8</v>
       </c>
+      <c r="J1131">
+        <v>0</v>
+      </c>
       <c r="K1131" t="s">
         <v>71</v>
       </c>
@@ -60056,6 +61224,9 @@
       <c r="I1132" t="s">
         <v>12</v>
       </c>
+      <c r="J1132">
+        <v>0</v>
+      </c>
       <c r="K1132" t="s">
         <v>71</v>
       </c>
@@ -60106,6 +61277,9 @@
       <c r="I1133" t="s">
         <v>12</v>
       </c>
+      <c r="J1133">
+        <v>0</v>
+      </c>
       <c r="K1133" t="s">
         <v>71</v>
       </c>
@@ -60156,6 +61330,9 @@
       <c r="I1134" t="s">
         <v>16</v>
       </c>
+      <c r="J1134">
+        <v>0</v>
+      </c>
       <c r="K1134" t="s">
         <v>71</v>
       </c>
@@ -60206,6 +61383,9 @@
       <c r="I1135" t="s">
         <v>17</v>
       </c>
+      <c r="J1135">
+        <v>0</v>
+      </c>
       <c r="K1135" t="s">
         <v>71</v>
       </c>
@@ -60256,6 +61436,9 @@
       <c r="I1136" t="s">
         <v>47</v>
       </c>
+      <c r="J1136">
+        <v>0</v>
+      </c>
       <c r="K1136" t="s">
         <v>71</v>
       </c>
@@ -60304,6 +61487,9 @@
         <v>5</v>
       </c>
       <c r="I1137" t="s">
+        <v>0</v>
+      </c>
+      <c r="J1137">
         <v>0</v>
       </c>
       <c r="K1137" t="s">
@@ -60356,6 +61542,9 @@
       <c r="I1138" t="s">
         <v>36</v>
       </c>
+      <c r="J1138">
+        <v>0</v>
+      </c>
       <c r="K1138" t="s">
         <v>71</v>
       </c>
@@ -60406,6 +61595,9 @@
       <c r="I1139" t="s">
         <v>1</v>
       </c>
+      <c r="J1139">
+        <v>0</v>
+      </c>
       <c r="K1139" t="s">
         <v>71</v>
       </c>
@@ -60456,6 +61648,9 @@
       <c r="I1140" t="s">
         <v>34</v>
       </c>
+      <c r="J1140">
+        <v>0</v>
+      </c>
       <c r="K1140" t="s">
         <v>71</v>
       </c>
@@ -60506,6 +61701,9 @@
       <c r="I1141" t="s">
         <v>38</v>
       </c>
+      <c r="J1141">
+        <v>0</v>
+      </c>
       <c r="K1141" t="s">
         <v>71</v>
       </c>
@@ -60556,6 +61754,9 @@
       <c r="I1142" t="s">
         <v>9</v>
       </c>
+      <c r="J1142">
+        <v>0</v>
+      </c>
       <c r="K1142" t="s">
         <v>71</v>
       </c>
@@ -60605,6 +61806,9 @@
       </c>
       <c r="I1143" t="s">
         <v>12</v>
+      </c>
+      <c r="J1143">
+        <v>0</v>
       </c>
       <c r="K1143" t="s">
         <v>71</v>

</xml_diff>